<commit_message>
new: "ACTRIS data" def., concepts for PID use
</commit_message>
<xml_diff>
--- a/ACTRIS_controlled_lists.xlsx
+++ b/ACTRIS_controlled_lists.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nilu365.sharepoint.com/sites/Project-ACTRIS/Shared Documents/WP2 - In-Situ/vocabulary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{E749C578-829D-4EB5-A142-7BC12B5C6B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30E9D88C-2E90-4E67-8652-9889B3448927}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{BF389FC4-FC65-4BA5-9E28-BDD5C3511B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{987A924B-8114-4DC5-9C66-4329D06AE180}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="26355" windowHeight="12630" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="2985" windowWidth="38700" windowHeight="15435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="controlled-terminology" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="171">
   <si>
     <t xml:space="preserve">ConceptScheme URI </t>
   </si>
@@ -449,10 +449,106 @@
     <t>RI-URBANS</t>
   </si>
   <si>
-    <t>2023-09-04T22:30:00+02:00</t>
+    <t>2023-09-05T19:00:00+02:00</t>
+  </si>
+  <si>
+    <t>ACTRIS_ctrl_lists:DOI</t>
+  </si>
+  <si>
+    <t>submission DOI</t>
+  </si>
+  <si>
+    <t>version DOI</t>
+  </si>
+  <si>
+    <t>concept DOI</t>
+  </si>
+  <si>
+    <t>collection DOI</t>
+  </si>
+  <si>
+    <t>Digital object identifier for a single data delivery from an identified instrument at an identified location. Used to document data production chain (provenance).</t>
+  </si>
+  <si>
+    <t>Digital object identifier pointing towards an assembly of DOI identified objects of any type. Often used to identify collections of data objects analysed for a publication.</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0003-3587-5926</t>
+  </si>
+  <si>
+    <t>Digital object identifier for a consistent set of data submissions from an identified instrument type and model at an identified location. Consistent means connected without known ruptures, e.g. changes in operating procedures. Used to identify exact version of a data stream in an analysis.</t>
+  </si>
+  <si>
+    <t>Glossary</t>
+  </si>
+  <si>
+    <t>ACTRIS data</t>
+  </si>
+  <si>
+    <t>ACTRIS_ctrl_lists:Glossary</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Glossary</t>
+  </si>
+  <si>
+    <t>ACTRIS_vocab</t>
+  </si>
+  <si>
+    <t>ACTRIS_vocab:ACTRISlabelled</t>
+  </si>
+  <si>
+    <t>ACTRIS data are data from observational or exploratory National Facilities complying with the procedures established within ACTRIS. ACTRIS data have received the "ACTRIS labelled" designator.</t>
+  </si>
+  <si>
+    <t>Identifiers used in ACTRIS.</t>
+  </si>
+  <si>
+    <t>identifier</t>
+  </si>
+  <si>
+    <t>ACTRIS_ctrl_lists:identifier</t>
+  </si>
+  <si>
+    <t>identifier use</t>
+  </si>
+  <si>
+    <t>Uses of persistent identifiers used in ACTRIS.</t>
+  </si>
+  <si>
+    <t>submission PID</t>
+  </si>
+  <si>
+    <t>version PID</t>
+  </si>
+  <si>
+    <t>concept PID</t>
+  </si>
+  <si>
+    <t>collection PID</t>
+  </si>
+  <si>
+    <t>ACTRIS_ctrl_lists:identifieruse</t>
+  </si>
+  <si>
+    <t>Persistent identifier for a single data delivery from an identified instrument at an identified location. Used to document data production chain (provenance).</t>
+  </si>
+  <si>
+    <t>Persistent identifier for a consistent set of data submissions from an identified instrument type and model at an identified location. Consistent means connected without known ruptures, e.g. changes in operating procedures. Used to identify exact version of a data stream in an analysis.</t>
+  </si>
+  <si>
+    <t>Persistent identifier representing all versions of a record. Here, record means consistent set of data submissions from an identified instrument type and model at an identified location. Used to identify all previous, current, and future versions of the record.</t>
+  </si>
+  <si>
+    <t>Persistent identifier pointing towards an assembly of PID identified objects of any type. Often used to identify collections of data objects analysed for a publication.</t>
+  </si>
+  <si>
+    <t>Digital object identifier representing all versions of a record. Here, record means consistent set of data submissions from an identified instrument type and model at an identified location. Used to identify all previous, current, and future versions of the record.</t>
   </si>
   <si>
     <t>https://vocabulary.actris.nilu.no/actris_controlled_lists/</t>
+  </si>
+  <si>
+    <t>https://vocabulary.actris.nilu.no/actris_vocab/</t>
   </si>
 </sst>
 </file>
@@ -462,7 +558,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -512,6 +608,19 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF0563C1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -621,11 +730,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -674,10 +785,21 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink 2" xfId="3" xr:uid="{AD1C3A76-3EA8-407A-B2AC-2A2C76B51742}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{5B150E8B-30AF-4D43-9F6A-886D70FEA9BC}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1057,12 +1179,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P98"/>
+  <dimension ref="A1:P115"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A1771" sqref="A1771"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1:D2"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1086,7 +1208,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>138</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -1097,53 +1219,56 @@
         <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>138</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
+      <c r="B3" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>6</v>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
+      <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>10</v>
@@ -1151,64 +1276,66 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B11" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B12" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B13" s="7" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B15" s="8" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="str">
-        <f>IF(ISBLANK($B15),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B15," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
-        <v/>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1217,7 +1344,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="str">
         <f>IF(ISBLANK($B17),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B17," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
         <v/>
@@ -1229,137 +1356,114 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="str">
+        <f>IF(ISBLANK($B19),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B19," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B20" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C20" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D20" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E20" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F20" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="G20" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="H20" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="I19" s="11" t="s">
+      <c r="I20" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="J19" s="11" t="s">
+      <c r="J20" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="K19" s="11" t="s">
+      <c r="K20" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="L19" s="11" t="s">
+      <c r="L20" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="M19" s="11" t="s">
+      <c r="M20" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="N19" s="11" t="s">
+      <c r="N20" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="O19" s="11" t="s">
+      <c r="O20" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="P19" s="11" t="s">
+      <c r="P20" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="12" t="str">
-        <f t="shared" ref="A20:A51" si="0">IF(ISBLANK($B20),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B20," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+    <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="str">
+        <f t="shared" ref="A21:A52" si="0">IF(ISBLANK($B21),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B21," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
         <v>ACTRIS_ctrl_lists:level</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B21" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C21" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D21" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="O20" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="P20" s="13"/>
-    </row>
-    <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v>ACTRIS_ctrl_lists:aggregate</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="16"/>
-      <c r="N21" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="O21" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="P21" s="18"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="O21" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="P21" s="13"/>
     </row>
     <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>ACTRIS_ctrl_lists:application</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
+        <v>ACTRIS_ctrl_lists:aggregate</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
       <c r="E22" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
       <c r="I22" s="18"/>
       <c r="J22" s="18"/>
       <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
       <c r="N22" s="19" t="s">
         <v>44</v>
       </c>
@@ -1371,48 +1475,48 @@
     <row r="23" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>ACTRIS_ctrl_lists:attribute</v>
-      </c>
-      <c r="B23" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="21"/>
-      <c r="D23" s="20"/>
+        <v>ACTRIS_ctrl_lists:application</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
       <c r="E23" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
       <c r="I23" s="18"/>
-      <c r="J23" s="20"/>
+      <c r="J23" s="18"/>
       <c r="K23" s="18"/>
-      <c r="L23" s="21"/>
-      <c r="M23" s="22"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
       <c r="N23" s="19" t="s">
         <v>44</v>
       </c>
       <c r="O23" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="P23" s="16"/>
+      <c r="P23" s="18"/>
     </row>
     <row r="24" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>ACTRIS_ctrl_lists:attributeType</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="C24" s="21"/>
-      <c r="D24" s="20"/>
+        <v>ACTRIS_ctrl_lists:attribute</v>
+      </c>
+      <c r="B24" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="31"/>
+      <c r="D24" s="30"/>
       <c r="E24" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
       <c r="I24" s="18"/>
       <c r="J24" s="20"/>
       <c r="K24" s="18"/>
@@ -1429,19 +1533,19 @@
     <row r="25" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>ACTRIS_ctrl_lists:collection</v>
-      </c>
-      <c r="B25" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" s="21"/>
-      <c r="D25" s="20"/>
+        <v>ACTRIS_ctrl_lists:attributeType</v>
+      </c>
+      <c r="B25" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="31"/>
+      <c r="D25" s="30"/>
       <c r="E25" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
       <c r="I25" s="18"/>
       <c r="J25" s="20"/>
       <c r="K25" s="18"/>
@@ -1458,48 +1562,48 @@
     <row r="26" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>ACTRIS_ctrl_lists:collectionHardware</v>
-      </c>
-      <c r="B26" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="20"/>
+        <v>ACTRIS_ctrl_lists:collection</v>
+      </c>
+      <c r="B26" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="31"/>
+      <c r="D26" s="30"/>
       <c r="E26" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
       <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
+      <c r="J26" s="20"/>
       <c r="K26" s="18"/>
-      <c r="L26" s="16"/>
-      <c r="M26" s="16"/>
+      <c r="L26" s="21"/>
+      <c r="M26" s="22"/>
       <c r="N26" s="19" t="s">
         <v>44</v>
       </c>
       <c r="O26" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="P26" s="18"/>
+      <c r="P26" s="16"/>
     </row>
     <row r="27" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>ACTRIS_ctrl_lists:collectionSession</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
+        <v>ACTRIS_ctrl_lists:collectionHardware</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="18"/>
+      <c r="D27" s="30"/>
       <c r="E27" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
       <c r="I27" s="18"/>
       <c r="J27" s="18"/>
       <c r="K27" s="18"/>
@@ -1516,19 +1620,19 @@
     <row r="28" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>ACTRIS_ctrl_lists:coverage</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
+        <v>ACTRIS_ctrl_lists:collectionSession</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
       <c r="E28" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
       <c r="I28" s="18"/>
       <c r="J28" s="18"/>
       <c r="K28" s="18"/>
@@ -1545,19 +1649,19 @@
     <row r="29" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>ACTRIS_ctrl_lists:dataset</v>
-      </c>
-      <c r="B29" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
+        <v>ACTRIS_ctrl_lists:coverage</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
       <c r="E29" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
       <c r="I29" s="18"/>
       <c r="J29" s="18"/>
       <c r="K29" s="18"/>
@@ -1574,19 +1678,19 @@
     <row r="30" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>ACTRIS_ctrl_lists:dimensionGroup</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
+        <v>ACTRIS_ctrl_lists:dataset</v>
+      </c>
+      <c r="B30" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
       <c r="E30" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
       <c r="I30" s="18"/>
       <c r="J30" s="18"/>
       <c r="K30" s="18"/>
@@ -1603,19 +1707,19 @@
     <row r="31" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>ACTRIS_ctrl_lists:document</v>
-      </c>
-      <c r="B31" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
+        <v>ACTRIS_ctrl_lists:dimensionGroup</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
       <c r="E31" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
       <c r="I31" s="18"/>
       <c r="J31" s="18"/>
       <c r="K31" s="18"/>
@@ -1632,19 +1736,19 @@
     <row r="32" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>ACTRIS_ctrl_lists:feature</v>
-      </c>
-      <c r="B32" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
+        <v>ACTRIS_ctrl_lists:document</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
       <c r="E32" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="F32" s="16"/>
-      <c r="G32" s="16"/>
-      <c r="H32" s="16"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
       <c r="I32" s="18"/>
       <c r="J32" s="18"/>
       <c r="K32" s="18"/>
@@ -1658,16 +1762,16 @@
       </c>
       <c r="P32" s="18"/>
     </row>
-    <row r="33" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>ACTRIS_ctrl_lists:featureType</v>
-      </c>
-      <c r="B33" s="17" t="s">
-        <v>59</v>
+        <v>ACTRIS_ctrl_lists:feature</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>58</v>
       </c>
       <c r="C33" s="18"/>
-      <c r="D33" s="17"/>
+      <c r="D33" s="18"/>
       <c r="E33" s="17" t="s">
         <v>47</v>
       </c>
@@ -1677,8 +1781,8 @@
       <c r="I33" s="18"/>
       <c r="J33" s="18"/>
       <c r="K33" s="18"/>
-      <c r="L33" s="18"/>
-      <c r="M33" s="18"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="16"/>
       <c r="N33" s="19" t="s">
         <v>44</v>
       </c>
@@ -1690,10 +1794,10 @@
     <row r="34" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>ACTRIS_ctrl_lists:fieldSession</v>
+        <v>ACTRIS_ctrl_lists:featureType</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C34" s="18"/>
       <c r="D34" s="17"/>
@@ -1719,10 +1823,10 @@
     <row r="35" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>ACTRIS_ctrl_lists:initiative</v>
+        <v>ACTRIS_ctrl_lists:fieldSession</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C35" s="18"/>
       <c r="D35" s="17"/>
@@ -1748,10 +1852,10 @@
     <row r="36" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>ACTRIS_ctrl_lists:metadata</v>
+        <v>ACTRIS_ctrl_lists:initiative</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C36" s="18"/>
       <c r="D36" s="17"/>
@@ -1777,10 +1881,10 @@
     <row r="37" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>ACTRIS_ctrl_lists:model</v>
+        <v>ACTRIS_ctrl_lists:metadata</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C37" s="18"/>
       <c r="D37" s="17"/>
@@ -1806,10 +1910,10 @@
     <row r="38" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>ACTRIS_ctrl_lists:nonGeographicDataset</v>
+        <v>ACTRIS_ctrl_lists:model</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C38" s="18"/>
       <c r="D38" s="17"/>
@@ -1835,10 +1939,10 @@
     <row r="39" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>ACTRIS_ctrl_lists:product</v>
+        <v>ACTRIS_ctrl_lists:nonGeographicDataset</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C39" s="18"/>
       <c r="D39" s="17"/>
@@ -1864,10 +1968,10 @@
     <row r="40" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>ACTRIS_ctrl_lists:propertyType</v>
+        <v>ACTRIS_ctrl_lists:product</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C40" s="18"/>
       <c r="D40" s="17"/>
@@ -1893,10 +1997,10 @@
     <row r="41" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>ACTRIS_ctrl_lists:repository</v>
+        <v>ACTRIS_ctrl_lists:propertyType</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C41" s="18"/>
       <c r="D41" s="17"/>
@@ -1922,10 +2026,10 @@
     <row r="42" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>ACTRIS_ctrl_lists:sample</v>
+        <v>ACTRIS_ctrl_lists:repository</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C42" s="18"/>
       <c r="D42" s="17"/>
@@ -1951,10 +2055,10 @@
     <row r="43" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>ACTRIS_ctrl_lists:series</v>
+        <v>ACTRIS_ctrl_lists:sample</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C43" s="18"/>
       <c r="D43" s="17"/>
@@ -1980,10 +2084,10 @@
     <row r="44" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>ACTRIS_ctrl_lists:service</v>
+        <v>ACTRIS_ctrl_lists:series</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C44" s="18"/>
       <c r="D44" s="17"/>
@@ -2009,10 +2113,10 @@
     <row r="45" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>ACTRIS_ctrl_lists:software</v>
+        <v>ACTRIS_ctrl_lists:service</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C45" s="18"/>
       <c r="D45" s="17"/>
@@ -2038,10 +2142,10 @@
     <row r="46" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>ACTRIS_ctrl_lists:tile</v>
+        <v>ACTRIS_ctrl_lists:software</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C46" s="18"/>
       <c r="D46" s="17"/>
@@ -2067,12 +2171,16 @@
     <row r="47" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="15" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B47" s="17"/>
+        <v>ACTRIS_ctrl_lists:tile</v>
+      </c>
+      <c r="B47" s="17" t="s">
+        <v>72</v>
+      </c>
       <c r="C47" s="18"/>
       <c r="D47" s="17"/>
-      <c r="E47" s="17"/>
+      <c r="E47" s="17" t="s">
+        <v>47</v>
+      </c>
       <c r="F47" s="18"/>
       <c r="G47" s="18"/>
       <c r="H47" s="18"/>
@@ -2081,8 +2189,12 @@
       <c r="K47" s="18"/>
       <c r="L47" s="18"/>
       <c r="M47" s="18"/>
-      <c r="N47" s="23"/>
-      <c r="O47" s="18"/>
+      <c r="N47" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="O47" s="18" t="s">
+        <v>45</v>
+      </c>
       <c r="P47" s="18"/>
     </row>
     <row r="48" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2106,79 +2218,69 @@
       <c r="O48" s="18"/>
       <c r="P48" s="18"/>
     </row>
-    <row r="49" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="12" t="str">
+    <row r="49" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B49" s="17"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="18"/>
+      <c r="I49" s="18"/>
+      <c r="J49" s="18"/>
+      <c r="K49" s="18"/>
+      <c r="L49" s="18"/>
+      <c r="M49" s="18"/>
+      <c r="N49" s="23"/>
+      <c r="O49" s="18"/>
+      <c r="P49" s="18"/>
+    </row>
+    <row r="50" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="12" t="str">
         <f t="shared" si="0"/>
         <v>ACTRIS_ctrl_lists:userroles</v>
       </c>
-      <c r="B49" s="13" t="s">
+      <c r="B50" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C49" s="13" t="s">
+      <c r="C50" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="D49" s="13" t="s">
+      <c r="D50" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
-      <c r="H49" s="13"/>
-      <c r="I49" s="13"/>
-      <c r="J49" s="13"/>
-      <c r="K49" s="13"/>
-      <c r="L49" s="13"/>
-      <c r="M49" s="13"/>
-      <c r="N49" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="O49" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="P49" s="13"/>
-    </row>
-    <row r="50" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v>ACTRIS_ctrl_lists:author</v>
-      </c>
-      <c r="B50" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="C50" s="18"/>
-      <c r="D50" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E50" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="F50" s="18"/>
-      <c r="G50" s="18"/>
-      <c r="H50" s="18"/>
-      <c r="I50" s="18"/>
-      <c r="J50" s="18"/>
-      <c r="K50" s="18"/>
-      <c r="L50" s="18"/>
-      <c r="M50" s="18"/>
-      <c r="N50" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="O50" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="P50" s="18"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="13"/>
+      <c r="J50" s="13"/>
+      <c r="K50" s="13"/>
+      <c r="L50" s="13"/>
+      <c r="M50" s="13"/>
+      <c r="N50" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="O50" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="P50" s="13"/>
     </row>
     <row r="51" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>ACTRIS_ctrl_lists:custodian</v>
+        <v>ACTRIS_ctrl_lists:author</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C51" s="18"/>
       <c r="D51" s="17" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E51" s="17" t="s">
         <v>78</v>
@@ -2201,15 +2303,15 @@
     </row>
     <row r="52" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="15" t="str">
-        <f t="shared" ref="A52:A84" si="1">IF(ISBLANK($B52),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B52," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
-        <v>ACTRIS_ctrl_lists:distributor</v>
+        <f t="shared" si="0"/>
+        <v>ACTRIS_ctrl_lists:custodian</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C52" s="18"/>
       <c r="D52" s="17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E52" s="17" t="s">
         <v>78</v>
@@ -2232,15 +2334,15 @@
     </row>
     <row r="53" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v>ACTRIS_ctrl_lists:originator</v>
+        <f t="shared" ref="A53:A97" si="1">IF(ISBLANK($B53),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B53," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <v>ACTRIS_ctrl_lists:distributor</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C53" s="18"/>
       <c r="D53" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E53" s="17" t="s">
         <v>78</v>
@@ -2264,14 +2366,14 @@
     <row r="54" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>ACTRIS_ctrl_lists:owner</v>
+        <v>ACTRIS_ctrl_lists:originator</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C54" s="18"/>
       <c r="D54" s="17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E54" s="17" t="s">
         <v>78</v>
@@ -2295,14 +2397,14 @@
     <row r="55" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>ACTRIS_ctrl_lists:pointOfContact</v>
+        <v>ACTRIS_ctrl_lists:owner</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C55" s="18"/>
       <c r="D55" s="17" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E55" s="17" t="s">
         <v>78</v>
@@ -2326,14 +2428,14 @@
     <row r="56" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>ACTRIS_ctrl_lists:principalInvestigator</v>
+        <v>ACTRIS_ctrl_lists:pointOfContact</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C56" s="18"/>
       <c r="D56" s="17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E56" s="17" t="s">
         <v>78</v>
@@ -2357,14 +2459,14 @@
     <row r="57" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>ACTRIS_ctrl_lists:processor</v>
+        <v>ACTRIS_ctrl_lists:principalInvestigator</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C57" s="18"/>
       <c r="D57" s="17" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E57" s="17" t="s">
         <v>78</v>
@@ -2388,14 +2490,14 @@
     <row r="58" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>ACTRIS_ctrl_lists:publisher</v>
+        <v>ACTRIS_ctrl_lists:processor</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C58" s="18"/>
       <c r="D58" s="17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E58" s="17" t="s">
         <v>78</v>
@@ -2419,14 +2521,14 @@
     <row r="59" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>ACTRIS_ctrl_lists:resourceProvider</v>
+        <v>ACTRIS_ctrl_lists:publisher</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C59" s="18"/>
       <c r="D59" s="17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E59" s="17" t="s">
         <v>78</v>
@@ -2450,14 +2552,14 @@
     <row r="60" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>ACTRIS_ctrl_lists:user</v>
+        <v>ACTRIS_ctrl_lists:resourceProvider</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C60" s="18"/>
       <c r="D60" s="17" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E60" s="17" t="s">
         <v>78</v>
@@ -2481,12 +2583,18 @@
     <row r="61" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="15" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B61" s="17"/>
+        <v>ACTRIS_ctrl_lists:user</v>
+      </c>
+      <c r="B61" s="17" t="s">
+        <v>97</v>
+      </c>
       <c r="C61" s="18"/>
-      <c r="D61" s="17"/>
-      <c r="E61" s="17"/>
+      <c r="D61" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="E61" s="17" t="s">
+        <v>78</v>
+      </c>
       <c r="F61" s="18"/>
       <c r="G61" s="18"/>
       <c r="H61" s="18"/>
@@ -2495,152 +2603,139 @@
       <c r="K61" s="18"/>
       <c r="L61" s="18"/>
       <c r="M61" s="18"/>
-      <c r="N61" s="23"/>
-      <c r="O61" s="18"/>
+      <c r="N61" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="O61" s="18" t="s">
+        <v>45</v>
+      </c>
       <c r="P61" s="18"/>
     </row>
-    <row r="62" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="12" t="str">
-        <f t="shared" si="1"/>
+    <row r="62" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="15"/>
+      <c r="B62" s="17"/>
+      <c r="C62" s="18"/>
+      <c r="D62" s="17"/>
+      <c r="E62" s="17"/>
+      <c r="F62" s="18"/>
+      <c r="G62" s="18"/>
+      <c r="H62" s="18"/>
+      <c r="I62" s="18"/>
+      <c r="J62" s="18"/>
+      <c r="K62" s="18"/>
+      <c r="L62" s="18"/>
+      <c r="M62" s="18"/>
+      <c r="N62" s="19"/>
+      <c r="O62" s="18"/>
+      <c r="P62" s="18"/>
+    </row>
+    <row r="63" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="12" t="str">
+        <f t="shared" ref="A63:A65" si="2">IF(ISBLANK($B63),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B63," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <v>ACTRIS_ctrl_lists:identifier</v>
+      </c>
+      <c r="B63" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="C63" s="13"/>
+      <c r="D63" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="E63" s="13"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="13"/>
+      <c r="H63" s="13"/>
+      <c r="I63" s="13"/>
+      <c r="J63" s="13"/>
+      <c r="K63" s="13"/>
+      <c r="L63" s="13"/>
+      <c r="M63" s="13"/>
+      <c r="N63" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="O63" s="13"/>
+      <c r="P63" s="13"/>
+    </row>
+    <row r="64" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="24" t="str">
+        <f t="shared" si="2"/>
         <v>ACTRIS_ctrl_lists:identifiertype</v>
       </c>
-      <c r="B62" s="13" t="s">
+      <c r="B64" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="C62" s="13" t="s">
+      <c r="C64" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="D62" s="13" t="s">
+      <c r="D64" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="E62" s="13"/>
-      <c r="F62" s="13"/>
-      <c r="G62" s="13"/>
-      <c r="H62" s="13"/>
-      <c r="I62" s="13"/>
-      <c r="J62" s="13"/>
-      <c r="K62" s="13"/>
-      <c r="L62" s="13"/>
-      <c r="M62" s="13"/>
-      <c r="N62" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="O62" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="P62" s="13"/>
-    </row>
-    <row r="63" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="15" t="str">
-        <f t="shared" si="1"/>
+      <c r="E64" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="F64" s="25"/>
+      <c r="G64" s="25"/>
+      <c r="H64" s="25"/>
+      <c r="I64" s="25"/>
+      <c r="J64" s="25"/>
+      <c r="K64" s="25"/>
+      <c r="L64" s="25"/>
+      <c r="M64" s="25"/>
+      <c r="N64" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="O64" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="P64" s="25"/>
+    </row>
+    <row r="65" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="27" t="str">
+        <f t="shared" si="2"/>
         <v>ACTRIS_ctrl_lists:DOI</v>
       </c>
-      <c r="B63" s="17" t="s">
+      <c r="B65" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="C63" s="18" t="s">
+      <c r="C65" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="D63" s="17"/>
-      <c r="E63" s="17" t="s">
+      <c r="D65" s="28"/>
+      <c r="E65" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="F63" s="18" t="s">
+      <c r="F65" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="G63" s="18"/>
-      <c r="H63" s="18"/>
-      <c r="I63" s="18"/>
-      <c r="J63" s="18"/>
-      <c r="K63" s="18"/>
-      <c r="L63" s="18"/>
-      <c r="M63" s="18"/>
-      <c r="N63" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="O63" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="P63" s="18"/>
-    </row>
-    <row r="64" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v>ACTRIS_ctrl_lists:handle</v>
-      </c>
-      <c r="B64" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="C64" s="18"/>
-      <c r="D64" s="17"/>
-      <c r="E64" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="F64" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="G64" s="18"/>
-      <c r="H64" s="18"/>
-      <c r="I64" s="18"/>
-      <c r="J64" s="18"/>
-      <c r="K64" s="18"/>
-      <c r="L64" s="18"/>
-      <c r="M64" s="18"/>
-      <c r="N64" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="O64" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="P64" s="18"/>
-    </row>
-    <row r="65" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v>ACTRIS_ctrl_lists:ePIC</v>
-      </c>
-      <c r="B65" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="C65" s="18"/>
-      <c r="D65" s="17"/>
-      <c r="E65" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="F65" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="G65" s="18"/>
-      <c r="H65" s="18"/>
-      <c r="I65" s="18"/>
-      <c r="J65" s="18"/>
-      <c r="K65" s="18"/>
-      <c r="L65" s="18"/>
-      <c r="M65" s="18"/>
-      <c r="N65" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="O65" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="P65" s="18"/>
+      <c r="G65" s="28"/>
+      <c r="H65" s="28"/>
+      <c r="I65" s="28"/>
+      <c r="J65" s="28"/>
+      <c r="K65" s="28"/>
+      <c r="L65" s="28"/>
+      <c r="M65" s="28"/>
+      <c r="N65" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="O65" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="P65" s="28"/>
     </row>
     <row r="66" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>ACTRIS_ctrl_lists:otherPID</v>
-      </c>
-      <c r="B66" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="C66" s="17" t="s">
-        <v>133</v>
-      </c>
+        <v>ACTRIS_ctrl_lists:submissionDOI</v>
+      </c>
+      <c r="B66" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="C66" s="18"/>
       <c r="D66" s="17" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="E66" s="17" t="s">
-        <v>104</v>
+        <v>138</v>
       </c>
       <c r="F66" s="18"/>
       <c r="G66" s="18"/>
@@ -2653,18 +2748,26 @@
       <c r="N66" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="O66" s="18"/>
+      <c r="O66" s="18" t="s">
+        <v>145</v>
+      </c>
       <c r="P66" s="18"/>
     </row>
     <row r="67" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="15" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B67" s="17"/>
+        <v>ACTRIS_ctrl_lists:versionDOI</v>
+      </c>
+      <c r="B67" s="17" t="s">
+        <v>140</v>
+      </c>
       <c r="C67" s="18"/>
-      <c r="D67" s="17"/>
-      <c r="E67" s="17"/>
+      <c r="D67" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="E67" s="17" t="s">
+        <v>138</v>
+      </c>
       <c r="F67" s="18"/>
       <c r="G67" s="18"/>
       <c r="H67" s="18"/>
@@ -2673,53 +2776,59 @@
       <c r="K67" s="18"/>
       <c r="L67" s="18"/>
       <c r="M67" s="18"/>
-      <c r="N67" s="23"/>
-      <c r="O67" s="18"/>
+      <c r="N67" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="O67" s="18" t="s">
+        <v>145</v>
+      </c>
       <c r="P67" s="18"/>
     </row>
-    <row r="68" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="12" t="str">
+    <row r="68" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>ACTRIS_ctrl_lists:framework</v>
-      </c>
-      <c r="B68" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="C68" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="D68" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="E68" s="13"/>
-      <c r="F68" s="13"/>
-      <c r="G68" s="13"/>
-      <c r="H68" s="13"/>
-      <c r="I68" s="13"/>
-      <c r="J68" s="13"/>
-      <c r="K68" s="13"/>
-      <c r="L68" s="13"/>
-      <c r="M68" s="13"/>
-      <c r="N68" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="O68" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="P68" s="13"/>
-    </row>
-    <row r="69" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>ACTRIS_ctrl_lists:conceptDOI</v>
+      </c>
+      <c r="B68" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="C68" s="18"/>
+      <c r="D68" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="E68" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="F68" s="18"/>
+      <c r="G68" s="18"/>
+      <c r="H68" s="18"/>
+      <c r="I68" s="18"/>
+      <c r="J68" s="18"/>
+      <c r="K68" s="18"/>
+      <c r="L68" s="18"/>
+      <c r="M68" s="18"/>
+      <c r="N68" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="O68" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="P68" s="18"/>
+    </row>
+    <row r="69" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>ACTRIS_ctrl_lists:ACTRIS</v>
+        <v>ACTRIS_ctrl_lists:collectionDOI</v>
       </c>
       <c r="B69" s="17" t="s">
-        <v>113</v>
+        <v>142</v>
       </c>
       <c r="C69" s="18"/>
-      <c r="D69" s="17"/>
+      <c r="D69" s="17" t="s">
+        <v>144</v>
+      </c>
       <c r="E69" s="17" t="s">
-        <v>114</v>
+        <v>138</v>
       </c>
       <c r="F69" s="18"/>
       <c r="G69" s="18"/>
@@ -2733,23 +2842,19 @@
         <v>44</v>
       </c>
       <c r="O69" s="18" t="s">
-        <v>45</v>
+        <v>145</v>
       </c>
       <c r="P69" s="18"/>
     </row>
-    <row r="70" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>ACTRIS_ctrl_lists:AMAP</v>
-      </c>
-      <c r="B70" s="17" t="s">
-        <v>115</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B70" s="17"/>
       <c r="C70" s="18"/>
       <c r="D70" s="17"/>
-      <c r="E70" s="17" t="s">
-        <v>114</v>
-      </c>
+      <c r="E70" s="17"/>
       <c r="F70" s="18"/>
       <c r="G70" s="18"/>
       <c r="H70" s="18"/>
@@ -2758,28 +2863,26 @@
       <c r="K70" s="18"/>
       <c r="L70" s="18"/>
       <c r="M70" s="18"/>
-      <c r="N70" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="O70" s="18" t="s">
-        <v>45</v>
-      </c>
+      <c r="N70" s="19"/>
+      <c r="O70" s="18"/>
       <c r="P70" s="18"/>
     </row>
-    <row r="71" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>ACTRIS_ctrl_lists:ARM</v>
+        <v>ACTRIS_ctrl_lists:handle</v>
       </c>
       <c r="B71" s="17" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="C71" s="18"/>
       <c r="D71" s="17"/>
       <c r="E71" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="F71" s="18"/>
+        <v>104</v>
+      </c>
+      <c r="F71" s="18" t="s">
+        <v>107</v>
+      </c>
       <c r="G71" s="18"/>
       <c r="H71" s="18"/>
       <c r="I71" s="18"/>
@@ -2795,20 +2898,22 @@
       </c>
       <c r="P71" s="18"/>
     </row>
-    <row r="72" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>ACTRIS_ctrl_lists:CAMP</v>
+        <v>ACTRIS_ctrl_lists:ePIC</v>
       </c>
       <c r="B72" s="17" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C72" s="18"/>
       <c r="D72" s="17"/>
       <c r="E72" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="F72" s="18"/>
+        <v>104</v>
+      </c>
+      <c r="F72" s="18" t="s">
+        <v>109</v>
+      </c>
       <c r="G72" s="18"/>
       <c r="H72" s="18"/>
       <c r="I72" s="18"/>
@@ -2824,18 +2929,22 @@
       </c>
       <c r="P72" s="18"/>
     </row>
-    <row r="73" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>ACTRIS_ctrl_lists:CLOUDNET</v>
-      </c>
-      <c r="B73" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="C73" s="18"/>
-      <c r="D73" s="17"/>
+        <v>ACTRIS_ctrl_lists:otherPID</v>
+      </c>
+      <c r="B73" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="C73" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D73" s="17" t="s">
+        <v>135</v>
+      </c>
       <c r="E73" s="17" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="F73" s="18"/>
       <c r="G73" s="18"/>
@@ -2848,52 +2957,54 @@
       <c r="N73" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="O73" s="18" t="s">
-        <v>45</v>
-      </c>
+      <c r="O73" s="18"/>
       <c r="P73" s="18"/>
     </row>
-    <row r="74" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v>ACTRIS_ctrl_lists:CREATE</v>
-      </c>
-      <c r="B74" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="C74" s="18"/>
-      <c r="D74" s="17"/>
-      <c r="E74" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="F74" s="18"/>
-      <c r="G74" s="18"/>
-      <c r="H74" s="18"/>
-      <c r="I74" s="18"/>
-      <c r="J74" s="18"/>
-      <c r="K74" s="18"/>
-      <c r="L74" s="18"/>
-      <c r="M74" s="18"/>
-      <c r="N74" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="O74" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="P74" s="18"/>
-    </row>
-    <row r="75" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="24" t="str">
+        <f t="shared" ref="A74:A78" si="3">IF(ISBLANK($B74),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B74," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <v>ACTRIS_ctrl_lists:identifieruse</v>
+      </c>
+      <c r="B74" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="C74" s="25"/>
+      <c r="D74" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="E74" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="F74" s="25"/>
+      <c r="G74" s="25"/>
+      <c r="H74" s="25"/>
+      <c r="I74" s="25"/>
+      <c r="J74" s="25"/>
+      <c r="K74" s="25"/>
+      <c r="L74" s="25"/>
+      <c r="M74" s="25"/>
+      <c r="N74" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="O74" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="P74" s="25"/>
+    </row>
+    <row r="75" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v>ACTRIS_ctrl_lists:EARLINET</v>
-      </c>
-      <c r="B75" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="C75" s="18"/>
-      <c r="D75" s="17"/>
+        <f t="shared" si="3"/>
+        <v>ACTRIS_ctrl_lists:submissionPID</v>
+      </c>
+      <c r="B75" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="C75" s="17"/>
+      <c r="D75" s="17" t="s">
+        <v>164</v>
+      </c>
       <c r="E75" s="17" t="s">
-        <v>114</v>
+        <v>163</v>
       </c>
       <c r="F75" s="18"/>
       <c r="G75" s="18"/>
@@ -2903,26 +3014,24 @@
       <c r="K75" s="18"/>
       <c r="L75" s="18"/>
       <c r="M75" s="18"/>
-      <c r="N75" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="O75" s="18" t="s">
-        <v>45</v>
-      </c>
+      <c r="N75" s="19"/>
+      <c r="O75" s="18"/>
       <c r="P75" s="18"/>
     </row>
-    <row r="76" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v>ACTRIS_ctrl_lists:EMEP</v>
-      </c>
-      <c r="B76" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="C76" s="18"/>
-      <c r="D76" s="17"/>
+        <f t="shared" si="3"/>
+        <v>ACTRIS_ctrl_lists:versionPID</v>
+      </c>
+      <c r="B76" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="C76" s="17"/>
+      <c r="D76" s="17" t="s">
+        <v>165</v>
+      </c>
       <c r="E76" s="17" t="s">
-        <v>114</v>
+        <v>163</v>
       </c>
       <c r="F76" s="18"/>
       <c r="G76" s="18"/>
@@ -2932,26 +3041,24 @@
       <c r="K76" s="18"/>
       <c r="L76" s="18"/>
       <c r="M76" s="18"/>
-      <c r="N76" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="O76" s="18" t="s">
-        <v>45</v>
-      </c>
+      <c r="N76" s="19"/>
+      <c r="O76" s="18"/>
       <c r="P76" s="18"/>
     </row>
-    <row r="77" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v>ACTRIS_ctrl_lists:EUROCHAMP</v>
-      </c>
-      <c r="B77" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="C77" s="18"/>
-      <c r="D77" s="17"/>
+        <f t="shared" si="3"/>
+        <v>ACTRIS_ctrl_lists:conceptPID</v>
+      </c>
+      <c r="B77" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="C77" s="17"/>
+      <c r="D77" s="17" t="s">
+        <v>166</v>
+      </c>
       <c r="E77" s="17" t="s">
-        <v>114</v>
+        <v>163</v>
       </c>
       <c r="F77" s="18"/>
       <c r="G77" s="18"/>
@@ -2961,26 +3068,24 @@
       <c r="K77" s="18"/>
       <c r="L77" s="18"/>
       <c r="M77" s="18"/>
-      <c r="N77" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="O77" s="18" t="s">
-        <v>45</v>
-      </c>
+      <c r="N77" s="19"/>
+      <c r="O77" s="18"/>
       <c r="P77" s="18"/>
     </row>
-    <row r="78" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v>ACTRIS_ctrl_lists:EUSAAR</v>
-      </c>
-      <c r="B78" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="C78" s="18"/>
-      <c r="D78" s="17"/>
+        <f t="shared" si="3"/>
+        <v>ACTRIS_ctrl_lists:collectionPID</v>
+      </c>
+      <c r="B78" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="C78" s="17"/>
+      <c r="D78" s="17" t="s">
+        <v>167</v>
+      </c>
       <c r="E78" s="17" t="s">
-        <v>114</v>
+        <v>163</v>
       </c>
       <c r="F78" s="18"/>
       <c r="G78" s="18"/>
@@ -2990,27 +3095,16 @@
       <c r="K78" s="18"/>
       <c r="L78" s="18"/>
       <c r="M78" s="18"/>
-      <c r="N78" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="O78" s="18" t="s">
-        <v>45</v>
-      </c>
+      <c r="N78" s="19"/>
+      <c r="O78" s="18"/>
       <c r="P78" s="18"/>
     </row>
-    <row r="79" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="15" t="str">
-        <f t="shared" si="1"/>
-        <v>ACTRIS_ctrl_lists:GAW-WDCA</v>
-      </c>
-      <c r="B79" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="C79" s="18"/>
+    <row r="79" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="15"/>
+      <c r="B79" s="18"/>
+      <c r="C79" s="17"/>
       <c r="D79" s="17"/>
-      <c r="E79" s="17" t="s">
-        <v>114</v>
-      </c>
+      <c r="E79" s="17"/>
       <c r="F79" s="18"/>
       <c r="G79" s="18"/>
       <c r="H79" s="18"/>
@@ -3019,27 +3113,19 @@
       <c r="K79" s="18"/>
       <c r="L79" s="18"/>
       <c r="M79" s="18"/>
-      <c r="N79" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="O79" s="18" t="s">
-        <v>45</v>
-      </c>
+      <c r="N79" s="19"/>
+      <c r="O79" s="18"/>
       <c r="P79" s="18"/>
     </row>
-    <row r="80" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>ACTRIS_ctrl_lists:GAW-WDCRG</v>
-      </c>
-      <c r="B80" s="17" t="s">
-        <v>125</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B80" s="17"/>
       <c r="C80" s="18"/>
       <c r="D80" s="17"/>
-      <c r="E80" s="17" t="s">
-        <v>114</v>
-      </c>
+      <c r="E80" s="17"/>
       <c r="F80" s="18"/>
       <c r="G80" s="18"/>
       <c r="H80" s="18"/>
@@ -3048,50 +3134,48 @@
       <c r="K80" s="18"/>
       <c r="L80" s="18"/>
       <c r="M80" s="18"/>
-      <c r="N80" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="O80" s="18" t="s">
-        <v>45</v>
-      </c>
+      <c r="N80" s="23"/>
+      <c r="O80" s="18"/>
       <c r="P80" s="18"/>
     </row>
-    <row r="81" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="15" t="str">
+    <row r="81" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="12" t="str">
         <f t="shared" si="1"/>
-        <v>ACTRIS_ctrl_lists:GUAN</v>
-      </c>
-      <c r="B81" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="C81" s="18"/>
-      <c r="D81" s="17"/>
-      <c r="E81" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="F81" s="18"/>
-      <c r="G81" s="18"/>
-      <c r="H81" s="18"/>
-      <c r="I81" s="18"/>
-      <c r="J81" s="18"/>
-      <c r="K81" s="18"/>
-      <c r="L81" s="18"/>
-      <c r="M81" s="18"/>
-      <c r="N81" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="O81" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="P81" s="18"/>
+        <v>ACTRIS_ctrl_lists:framework</v>
+      </c>
+      <c r="B81" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C81" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D81" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="E81" s="13"/>
+      <c r="F81" s="13"/>
+      <c r="G81" s="13"/>
+      <c r="H81" s="13"/>
+      <c r="I81" s="13"/>
+      <c r="J81" s="13"/>
+      <c r="K81" s="13"/>
+      <c r="L81" s="13"/>
+      <c r="M81" s="13"/>
+      <c r="N81" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="O81" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="P81" s="13"/>
     </row>
     <row r="82" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>ACTRIS_ctrl_lists:HELCOM</v>
+        <v>ACTRIS_ctrl_lists:ACTRIS</v>
       </c>
       <c r="B82" s="17" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="C82" s="18"/>
       <c r="D82" s="17"/>
@@ -3117,10 +3201,10 @@
     <row r="83" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>ACTRIS_ctrl_lists:NDACC</v>
+        <v>ACTRIS_ctrl_lists:AMAP</v>
       </c>
       <c r="B83" s="17" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="C83" s="18"/>
       <c r="D83" s="17"/>
@@ -3146,10 +3230,10 @@
     <row r="84" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="15" t="str">
         <f t="shared" si="1"/>
-        <v>ACTRIS_ctrl_lists:NILU</v>
+        <v>ACTRIS_ctrl_lists:ARM</v>
       </c>
       <c r="B84" s="17" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="C84" s="18"/>
       <c r="D84" s="17"/>
@@ -3172,13 +3256,13 @@
       </c>
       <c r="P84" s="18"/>
     </row>
-    <row r="85" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="15" t="str">
-        <f t="shared" ref="A85:A98" si="2">IF(ISBLANK($B85),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B85," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
-        <v>ACTRIS_ctrl_lists:NOAA-ESRL</v>
+        <f t="shared" si="1"/>
+        <v>ACTRIS_ctrl_lists:CAMP</v>
       </c>
       <c r="B85" s="17" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="C85" s="18"/>
       <c r="D85" s="17"/>
@@ -3201,13 +3285,13 @@
       </c>
       <c r="P85" s="18"/>
     </row>
-    <row r="86" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v>ACTRIS_ctrl_lists:GALION</v>
+        <f t="shared" si="1"/>
+        <v>ACTRIS_ctrl_lists:CLOUDNET</v>
       </c>
       <c r="B86" s="17" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="C86" s="18"/>
       <c r="D86" s="17"/>
@@ -3225,16 +3309,18 @@
       <c r="N86" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="O86" s="18"/>
+      <c r="O86" s="18" t="s">
+        <v>45</v>
+      </c>
       <c r="P86" s="18"/>
     </row>
-    <row r="87" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v>ACTRIS_ctrl_lists:AERONET</v>
+        <f t="shared" si="1"/>
+        <v>ACTRIS_ctrl_lists:CREATE</v>
       </c>
       <c r="B87" s="17" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="C87" s="18"/>
       <c r="D87" s="17"/>
@@ -3252,16 +3338,18 @@
       <c r="N87" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="O87" s="18"/>
+      <c r="O87" s="18" t="s">
+        <v>45</v>
+      </c>
       <c r="P87" s="18"/>
     </row>
-    <row r="88" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v>ACTRIS_ctrl_lists:RI-URBANS</v>
+        <f t="shared" si="1"/>
+        <v>ACTRIS_ctrl_lists:EARLINET</v>
       </c>
       <c r="B88" s="17" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="C88" s="18"/>
       <c r="D88" s="17"/>
@@ -3279,18 +3367,24 @@
       <c r="N88" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="O88" s="18"/>
+      <c r="O88" s="18" t="s">
+        <v>45</v>
+      </c>
       <c r="P88" s="18"/>
     </row>
-    <row r="89" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="B89" s="17"/>
+        <f t="shared" si="1"/>
+        <v>ACTRIS_ctrl_lists:EMEP</v>
+      </c>
+      <c r="B89" s="17" t="s">
+        <v>121</v>
+      </c>
       <c r="C89" s="18"/>
       <c r="D89" s="17"/>
-      <c r="E89" s="17"/>
+      <c r="E89" s="17" t="s">
+        <v>114</v>
+      </c>
       <c r="F89" s="18"/>
       <c r="G89" s="18"/>
       <c r="H89" s="18"/>
@@ -3299,19 +3393,27 @@
       <c r="K89" s="18"/>
       <c r="L89" s="18"/>
       <c r="M89" s="18"/>
-      <c r="N89" s="23"/>
-      <c r="O89" s="18"/>
+      <c r="N89" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="O89" s="18" t="s">
+        <v>45</v>
+      </c>
       <c r="P89" s="18"/>
     </row>
-    <row r="90" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="B90" s="17"/>
+        <f t="shared" si="1"/>
+        <v>ACTRIS_ctrl_lists:EUROCHAMP</v>
+      </c>
+      <c r="B90" s="17" t="s">
+        <v>122</v>
+      </c>
       <c r="C90" s="18"/>
       <c r="D90" s="17"/>
-      <c r="E90" s="17"/>
+      <c r="E90" s="17" t="s">
+        <v>114</v>
+      </c>
       <c r="F90" s="18"/>
       <c r="G90" s="18"/>
       <c r="H90" s="18"/>
@@ -3320,19 +3422,27 @@
       <c r="K90" s="18"/>
       <c r="L90" s="18"/>
       <c r="M90" s="18"/>
-      <c r="N90" s="23"/>
-      <c r="O90" s="18"/>
+      <c r="N90" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="O90" s="18" t="s">
+        <v>45</v>
+      </c>
       <c r="P90" s="18"/>
     </row>
-    <row r="91" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="B91" s="17"/>
+        <f t="shared" si="1"/>
+        <v>ACTRIS_ctrl_lists:EUSAAR</v>
+      </c>
+      <c r="B91" s="17" t="s">
+        <v>123</v>
+      </c>
       <c r="C91" s="18"/>
       <c r="D91" s="17"/>
-      <c r="E91" s="17"/>
+      <c r="E91" s="17" t="s">
+        <v>114</v>
+      </c>
       <c r="F91" s="18"/>
       <c r="G91" s="18"/>
       <c r="H91" s="18"/>
@@ -3341,19 +3451,27 @@
       <c r="K91" s="18"/>
       <c r="L91" s="18"/>
       <c r="M91" s="18"/>
-      <c r="N91" s="23"/>
-      <c r="O91" s="18"/>
+      <c r="N91" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="O91" s="18" t="s">
+        <v>45</v>
+      </c>
       <c r="P91" s="18"/>
     </row>
-    <row r="92" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="B92" s="17"/>
+        <f t="shared" si="1"/>
+        <v>ACTRIS_ctrl_lists:GAW-WDCA</v>
+      </c>
+      <c r="B92" s="17" t="s">
+        <v>124</v>
+      </c>
       <c r="C92" s="18"/>
       <c r="D92" s="17"/>
-      <c r="E92" s="17"/>
+      <c r="E92" s="17" t="s">
+        <v>114</v>
+      </c>
       <c r="F92" s="18"/>
       <c r="G92" s="18"/>
       <c r="H92" s="18"/>
@@ -3362,19 +3480,27 @@
       <c r="K92" s="18"/>
       <c r="L92" s="18"/>
       <c r="M92" s="18"/>
-      <c r="N92" s="23"/>
-      <c r="O92" s="18"/>
+      <c r="N92" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="O92" s="18" t="s">
+        <v>45</v>
+      </c>
       <c r="P92" s="18"/>
     </row>
-    <row r="93" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="B93" s="17"/>
+        <f t="shared" si="1"/>
+        <v>ACTRIS_ctrl_lists:GAW-WDCRG</v>
+      </c>
+      <c r="B93" s="17" t="s">
+        <v>125</v>
+      </c>
       <c r="C93" s="18"/>
       <c r="D93" s="17"/>
-      <c r="E93" s="17"/>
+      <c r="E93" s="17" t="s">
+        <v>114</v>
+      </c>
       <c r="F93" s="18"/>
       <c r="G93" s="18"/>
       <c r="H93" s="18"/>
@@ -3383,88 +3509,114 @@
       <c r="K93" s="18"/>
       <c r="L93" s="18"/>
       <c r="M93" s="18"/>
-      <c r="N93" s="23"/>
-      <c r="O93" s="18"/>
+      <c r="N93" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="O93" s="18" t="s">
+        <v>45</v>
+      </c>
       <c r="P93" s="18"/>
     </row>
-    <row r="94" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="12" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="B94" s="13"/>
-      <c r="C94" s="13"/>
-      <c r="D94" s="13"/>
-      <c r="E94" s="13"/>
-      <c r="F94" s="13"/>
-      <c r="G94" s="13"/>
-      <c r="H94" s="13"/>
-      <c r="I94" s="13"/>
-      <c r="J94" s="13"/>
-      <c r="K94" s="13"/>
-      <c r="L94" s="13"/>
-      <c r="M94" s="13"/>
-      <c r="N94" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="O94" s="13"/>
-      <c r="P94" s="13"/>
-    </row>
-    <row r="95" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="24" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="B95" s="25"/>
-      <c r="C95" s="25"/>
-      <c r="D95" s="25"/>
-      <c r="E95" s="25"/>
-      <c r="F95" s="25"/>
-      <c r="G95" s="25"/>
-      <c r="H95" s="25"/>
-      <c r="I95" s="25"/>
-      <c r="J95" s="25"/>
-      <c r="K95" s="25"/>
-      <c r="L95" s="25"/>
-      <c r="M95" s="25"/>
-      <c r="N95" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="O95" s="25"/>
-      <c r="P95" s="25"/>
-    </row>
-    <row r="96" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="27" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="B96" s="28"/>
-      <c r="C96" s="28"/>
-      <c r="D96" s="28"/>
-      <c r="E96" s="28"/>
-      <c r="F96" s="28"/>
-      <c r="G96" s="28"/>
-      <c r="H96" s="28"/>
-      <c r="I96" s="28"/>
-      <c r="J96" s="28"/>
-      <c r="K96" s="28"/>
-      <c r="L96" s="28"/>
-      <c r="M96" s="28"/>
-      <c r="N96" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="O96" s="28"/>
-      <c r="P96" s="28"/>
-    </row>
-    <row r="97" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v>ACTRIS_ctrl_lists:GUAN</v>
+      </c>
+      <c r="B94" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="C94" s="18"/>
+      <c r="D94" s="17"/>
+      <c r="E94" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="F94" s="18"/>
+      <c r="G94" s="18"/>
+      <c r="H94" s="18"/>
+      <c r="I94" s="18"/>
+      <c r="J94" s="18"/>
+      <c r="K94" s="18"/>
+      <c r="L94" s="18"/>
+      <c r="M94" s="18"/>
+      <c r="N94" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="O94" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="P94" s="18"/>
+    </row>
+    <row r="95" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v>ACTRIS_ctrl_lists:HELCOM</v>
+      </c>
+      <c r="B95" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="C95" s="18"/>
+      <c r="D95" s="17"/>
+      <c r="E95" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="F95" s="18"/>
+      <c r="G95" s="18"/>
+      <c r="H95" s="18"/>
+      <c r="I95" s="18"/>
+      <c r="J95" s="18"/>
+      <c r="K95" s="18"/>
+      <c r="L95" s="18"/>
+      <c r="M95" s="18"/>
+      <c r="N95" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="O95" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="P95" s="18"/>
+    </row>
+    <row r="96" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="15" t="str">
+        <f t="shared" si="1"/>
+        <v>ACTRIS_ctrl_lists:NDACC</v>
+      </c>
+      <c r="B96" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="C96" s="18"/>
+      <c r="D96" s="17"/>
+      <c r="E96" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="F96" s="18"/>
+      <c r="G96" s="18"/>
+      <c r="H96" s="18"/>
+      <c r="I96" s="18"/>
+      <c r="J96" s="18"/>
+      <c r="K96" s="18"/>
+      <c r="L96" s="18"/>
+      <c r="M96" s="18"/>
+      <c r="N96" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="O96" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="P96" s="18"/>
+    </row>
+    <row r="97" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="B97" s="17"/>
+        <f t="shared" si="1"/>
+        <v>ACTRIS_ctrl_lists:NILU</v>
+      </c>
+      <c r="B97" s="17" t="s">
+        <v>129</v>
+      </c>
       <c r="C97" s="18"/>
       <c r="D97" s="17"/>
-      <c r="E97" s="17"/>
+      <c r="E97" s="17" t="s">
+        <v>114</v>
+      </c>
       <c r="F97" s="18"/>
       <c r="G97" s="18"/>
       <c r="H97" s="18"/>
@@ -3473,21 +3625,27 @@
       <c r="K97" s="18"/>
       <c r="L97" s="18"/>
       <c r="M97" s="18"/>
-      <c r="N97" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="O97" s="23"/>
+      <c r="N97" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="O97" s="18" t="s">
+        <v>45</v>
+      </c>
       <c r="P97" s="18"/>
     </row>
     <row r="98" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="15" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="B98" s="18"/>
+        <f t="shared" ref="A98:A115" si="4">IF(ISBLANK($B98),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B98," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <v>ACTRIS_ctrl_lists:NOAA-ESRL</v>
+      </c>
+      <c r="B98" s="17" t="s">
+        <v>130</v>
+      </c>
       <c r="C98" s="18"/>
       <c r="D98" s="17"/>
-      <c r="E98" s="17"/>
+      <c r="E98" s="17" t="s">
+        <v>114</v>
+      </c>
       <c r="F98" s="18"/>
       <c r="G98" s="18"/>
       <c r="H98" s="18"/>
@@ -3496,160 +3654,547 @@
       <c r="K98" s="18"/>
       <c r="L98" s="18"/>
       <c r="M98" s="18"/>
-      <c r="N98" s="23"/>
-      <c r="O98" s="23"/>
+      <c r="N98" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="O98" s="18" t="s">
+        <v>45</v>
+      </c>
       <c r="P98" s="18"/>
+    </row>
+    <row r="99" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v>ACTRIS_ctrl_lists:GALION</v>
+      </c>
+      <c r="B99" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="C99" s="18"/>
+      <c r="D99" s="17"/>
+      <c r="E99" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="F99" s="18"/>
+      <c r="G99" s="18"/>
+      <c r="H99" s="18"/>
+      <c r="I99" s="18"/>
+      <c r="J99" s="18"/>
+      <c r="K99" s="18"/>
+      <c r="L99" s="18"/>
+      <c r="M99" s="18"/>
+      <c r="N99" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="O99" s="18"/>
+      <c r="P99" s="18"/>
+    </row>
+    <row r="100" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v>ACTRIS_ctrl_lists:AERONET</v>
+      </c>
+      <c r="B100" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="C100" s="18"/>
+      <c r="D100" s="17"/>
+      <c r="E100" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="F100" s="18"/>
+      <c r="G100" s="18"/>
+      <c r="H100" s="18"/>
+      <c r="I100" s="18"/>
+      <c r="J100" s="18"/>
+      <c r="K100" s="18"/>
+      <c r="L100" s="18"/>
+      <c r="M100" s="18"/>
+      <c r="N100" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="O100" s="18"/>
+      <c r="P100" s="18"/>
+    </row>
+    <row r="101" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v>ACTRIS_ctrl_lists:RI-URBANS</v>
+      </c>
+      <c r="B101" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="C101" s="18"/>
+      <c r="D101" s="17"/>
+      <c r="E101" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="F101" s="18"/>
+      <c r="G101" s="18"/>
+      <c r="H101" s="18"/>
+      <c r="I101" s="18"/>
+      <c r="J101" s="18"/>
+      <c r="K101" s="18"/>
+      <c r="L101" s="18"/>
+      <c r="M101" s="18"/>
+      <c r="N101" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="O101" s="18"/>
+      <c r="P101" s="18"/>
+    </row>
+    <row r="102" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B102" s="17"/>
+      <c r="C102" s="18"/>
+      <c r="D102" s="17"/>
+      <c r="E102" s="17"/>
+      <c r="F102" s="18"/>
+      <c r="G102" s="18"/>
+      <c r="H102" s="18"/>
+      <c r="I102" s="18"/>
+      <c r="J102" s="18"/>
+      <c r="K102" s="18"/>
+      <c r="L102" s="18"/>
+      <c r="M102" s="18"/>
+      <c r="N102" s="23"/>
+      <c r="O102" s="18"/>
+      <c r="P102" s="18"/>
+    </row>
+    <row r="103" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="15"/>
+      <c r="B103" s="17"/>
+      <c r="C103" s="18"/>
+      <c r="D103" s="17"/>
+      <c r="E103" s="17"/>
+      <c r="F103" s="18"/>
+      <c r="G103" s="18"/>
+      <c r="H103" s="18"/>
+      <c r="I103" s="18"/>
+      <c r="J103" s="18"/>
+      <c r="K103" s="18"/>
+      <c r="L103" s="18"/>
+      <c r="M103" s="18"/>
+      <c r="N103" s="23"/>
+      <c r="O103" s="18"/>
+      <c r="P103" s="18"/>
+    </row>
+    <row r="104" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="12" t="str">
+        <f t="shared" ref="A104:A105" si="5">IF(ISBLANK($B104),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B104," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <v>ACTRIS_ctrl_lists:Glossary</v>
+      </c>
+      <c r="B104" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="C104" s="13"/>
+      <c r="D104" s="13"/>
+      <c r="E104" s="13"/>
+      <c r="F104" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="G104" s="13"/>
+      <c r="H104" s="13"/>
+      <c r="I104" s="13"/>
+      <c r="J104" s="13"/>
+      <c r="K104" s="13"/>
+      <c r="L104" s="13"/>
+      <c r="M104" s="13"/>
+      <c r="N104" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="O104" s="13"/>
+      <c r="P104" s="13"/>
+    </row>
+    <row r="105" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="15" t="str">
+        <f t="shared" si="5"/>
+        <v>ACTRIS_ctrl_lists:ACTRISdata</v>
+      </c>
+      <c r="B105" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="C105" s="18"/>
+      <c r="D105" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="E105" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="F105" s="18"/>
+      <c r="G105" s="18"/>
+      <c r="H105" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="I105" s="18"/>
+      <c r="J105" s="18"/>
+      <c r="K105" s="18"/>
+      <c r="L105" s="18"/>
+      <c r="M105" s="18"/>
+      <c r="N105" s="23"/>
+      <c r="O105" s="18"/>
+      <c r="P105" s="18"/>
+    </row>
+    <row r="106" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="15"/>
+      <c r="B106" s="17"/>
+      <c r="C106" s="18"/>
+      <c r="D106" s="17"/>
+      <c r="E106" s="17"/>
+      <c r="F106" s="18"/>
+      <c r="G106" s="18"/>
+      <c r="H106" s="18"/>
+      <c r="I106" s="18"/>
+      <c r="J106" s="18"/>
+      <c r="K106" s="18"/>
+      <c r="L106" s="18"/>
+      <c r="M106" s="18"/>
+      <c r="N106" s="23"/>
+      <c r="O106" s="18"/>
+      <c r="P106" s="18"/>
+    </row>
+    <row r="107" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B107" s="17"/>
+      <c r="C107" s="18"/>
+      <c r="D107" s="17"/>
+      <c r="E107" s="17"/>
+      <c r="F107" s="18"/>
+      <c r="G107" s="18"/>
+      <c r="H107" s="18"/>
+      <c r="I107" s="18"/>
+      <c r="J107" s="18"/>
+      <c r="K107" s="18"/>
+      <c r="L107" s="18"/>
+      <c r="M107" s="18"/>
+      <c r="N107" s="23"/>
+      <c r="O107" s="18"/>
+      <c r="P107" s="18"/>
+    </row>
+    <row r="108" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B108" s="17"/>
+      <c r="C108" s="18"/>
+      <c r="D108" s="17"/>
+      <c r="E108" s="17"/>
+      <c r="F108" s="18"/>
+      <c r="G108" s="18"/>
+      <c r="H108" s="18"/>
+      <c r="I108" s="18"/>
+      <c r="J108" s="18"/>
+      <c r="K108" s="18"/>
+      <c r="L108" s="18"/>
+      <c r="M108" s="18"/>
+      <c r="N108" s="23"/>
+      <c r="O108" s="18"/>
+      <c r="P108" s="18"/>
+    </row>
+    <row r="109" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B109" s="17"/>
+      <c r="C109" s="18"/>
+      <c r="D109" s="17"/>
+      <c r="E109" s="17"/>
+      <c r="F109" s="18"/>
+      <c r="G109" s="18"/>
+      <c r="H109" s="18"/>
+      <c r="I109" s="18"/>
+      <c r="J109" s="18"/>
+      <c r="K109" s="18"/>
+      <c r="L109" s="18"/>
+      <c r="M109" s="18"/>
+      <c r="N109" s="23"/>
+      <c r="O109" s="18"/>
+      <c r="P109" s="18"/>
+    </row>
+    <row r="110" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B110" s="17"/>
+      <c r="C110" s="18"/>
+      <c r="D110" s="17"/>
+      <c r="E110" s="17"/>
+      <c r="F110" s="18"/>
+      <c r="G110" s="18"/>
+      <c r="H110" s="18"/>
+      <c r="I110" s="18"/>
+      <c r="J110" s="18"/>
+      <c r="K110" s="18"/>
+      <c r="L110" s="18"/>
+      <c r="M110" s="18"/>
+      <c r="N110" s="23"/>
+      <c r="O110" s="18"/>
+      <c r="P110" s="18"/>
+    </row>
+    <row r="111" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="12" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B111" s="13"/>
+      <c r="C111" s="13"/>
+      <c r="D111" s="13"/>
+      <c r="E111" s="13"/>
+      <c r="F111" s="13"/>
+      <c r="G111" s="13"/>
+      <c r="H111" s="13"/>
+      <c r="I111" s="13"/>
+      <c r="J111" s="13"/>
+      <c r="K111" s="13"/>
+      <c r="L111" s="13"/>
+      <c r="M111" s="13"/>
+      <c r="N111" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="O111" s="13"/>
+      <c r="P111" s="13"/>
+    </row>
+    <row r="112" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="24" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B112" s="25"/>
+      <c r="C112" s="25"/>
+      <c r="D112" s="25"/>
+      <c r="E112" s="25"/>
+      <c r="F112" s="25"/>
+      <c r="G112" s="25"/>
+      <c r="H112" s="25"/>
+      <c r="I112" s="25"/>
+      <c r="J112" s="25"/>
+      <c r="K112" s="25"/>
+      <c r="L112" s="25"/>
+      <c r="M112" s="25"/>
+      <c r="N112" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="O112" s="25"/>
+      <c r="P112" s="25"/>
+    </row>
+    <row r="113" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="27" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B113" s="28"/>
+      <c r="C113" s="28"/>
+      <c r="D113" s="28"/>
+      <c r="E113" s="28"/>
+      <c r="F113" s="28"/>
+      <c r="G113" s="28"/>
+      <c r="H113" s="28"/>
+      <c r="I113" s="28"/>
+      <c r="J113" s="28"/>
+      <c r="K113" s="28"/>
+      <c r="L113" s="28"/>
+      <c r="M113" s="28"/>
+      <c r="N113" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="O113" s="28"/>
+      <c r="P113" s="28"/>
+    </row>
+    <row r="114" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B114" s="17"/>
+      <c r="C114" s="18"/>
+      <c r="D114" s="17"/>
+      <c r="E114" s="17"/>
+      <c r="F114" s="18"/>
+      <c r="G114" s="18"/>
+      <c r="H114" s="18"/>
+      <c r="I114" s="18"/>
+      <c r="J114" s="18"/>
+      <c r="K114" s="18"/>
+      <c r="L114" s="18"/>
+      <c r="M114" s="18"/>
+      <c r="N114" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="O114" s="23"/>
+      <c r="P114" s="18"/>
+    </row>
+    <row r="115" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B115" s="18"/>
+      <c r="C115" s="18"/>
+      <c r="D115" s="17"/>
+      <c r="E115" s="17"/>
+      <c r="F115" s="18"/>
+      <c r="G115" s="18"/>
+      <c r="H115" s="18"/>
+      <c r="I115" s="18"/>
+      <c r="J115" s="18"/>
+      <c r="K115" s="18"/>
+      <c r="L115" s="18"/>
+      <c r="M115" s="18"/>
+      <c r="N115" s="23"/>
+      <c r="O115" s="23"/>
+      <c r="P115" s="18"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B9" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B10" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="O20" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="N21" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="O21" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="N22" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="O22" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="N23" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="O23" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="N24" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="O24" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="N25" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="O25" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="N26" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="O26" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="N27" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="O27" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="N28" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="O28" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="N29" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="O29" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="N30" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="O30" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="N31" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="O31" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="N32" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="O32" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="N33" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="O33" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="N34" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="O34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="N35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="O35" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="N36" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="O36" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="N37" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="O37" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="N38" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="O38" r:id="rId41" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="N39" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="O39" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="N40" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="O40" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="N41" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="O41" r:id="rId47" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="N42" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="O42" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="N43" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="O43" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="N44" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="O44" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="N45" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="O45" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="N46" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="O46" r:id="rId57" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="O49" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="N50" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="O50" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="N51" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="O51" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="N52" r:id="rId63" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="O52" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="N53" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="O53" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="N54" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="O54" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="N55" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="O55" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="N56" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="O56" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="N57" r:id="rId73" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="O57" r:id="rId74" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="N58" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="O58" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="N59" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="O59" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="N60" r:id="rId79" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="O60" r:id="rId80" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="O62" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="F63" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="N63" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="O63" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="F64" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="N64" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="O64" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="F65" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="N65" r:id="rId89" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="O65" r:id="rId90" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="O68" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="N69" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="O69" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="N70" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="O70" r:id="rId95" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="N71" r:id="rId96" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="O71" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="N72" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="O72" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="N73" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="O73" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
-    <hyperlink ref="N74" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="O74" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
-    <hyperlink ref="N75" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="O75" r:id="rId105" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
-    <hyperlink ref="N76" r:id="rId106" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="O76" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
-    <hyperlink ref="N77" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="O77" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
-    <hyperlink ref="N78" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="O78" r:id="rId111" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
-    <hyperlink ref="N79" r:id="rId112" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="O79" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
-    <hyperlink ref="N80" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="O80" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
-    <hyperlink ref="N81" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
-    <hyperlink ref="O81" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
-    <hyperlink ref="N82" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
-    <hyperlink ref="O82" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
-    <hyperlink ref="N83" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
-    <hyperlink ref="O83" r:id="rId121" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
-    <hyperlink ref="N84" r:id="rId122" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
-    <hyperlink ref="O84" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
-    <hyperlink ref="N85" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
-    <hyperlink ref="O85" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
-    <hyperlink ref="N95" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
-    <hyperlink ref="N96" r:id="rId127" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
-    <hyperlink ref="N97" r:id="rId128" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
-    <hyperlink ref="N66" r:id="rId129" xr:uid="{9AF6E984-1653-430E-A3FB-A3D26D9878D9}"/>
-    <hyperlink ref="N86:N88" r:id="rId130" display="https://orcid.org/0000-0002-3380-3470" xr:uid="{C0237BC4-BA79-4297-A3EA-35626BCC8ACE}"/>
-    <hyperlink ref="B1" r:id="rId131" display="https://vocabulary" xr:uid="{DBE5C11C-DF9F-43C7-9A78-7575095D5440}"/>
-    <hyperlink ref="C2" r:id="rId132" display="https://vocabulary" xr:uid="{BD068CBD-4199-460C-860D-0F9DAE966750}"/>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B10" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B11" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="O21" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="N22" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="O22" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="N23" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="O23" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="N24" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="O24" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="N25" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="O25" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="N26" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="O26" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="N27" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="O27" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="N28" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="O28" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="N29" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="O29" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="N30" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="O30" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="N31" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="O31" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="N32" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="O32" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="N33" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="O33" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="N34" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="O34" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="N35" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="O35" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="N36" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="O36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="N37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="O37" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="N38" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="O38" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="N39" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="O39" r:id="rId41" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="N40" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="O40" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="N41" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="O41" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="N42" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="O42" r:id="rId47" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="N43" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="O43" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="N44" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="O44" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="N45" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="O45" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="N46" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="O46" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="N47" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="O47" r:id="rId57" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="O50" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="N51" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="O51" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="N52" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="O52" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="N53" r:id="rId63" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="O53" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="N54" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="O54" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="N55" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="O55" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="N56" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="O56" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="N57" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="O57" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="N58" r:id="rId73" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="O58" r:id="rId74" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="N59" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="O59" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="N60" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="O60" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="N61" r:id="rId79" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="O61" r:id="rId80" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="F71" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="N71" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="O71" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="F72" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="N72" r:id="rId85" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="O72" r:id="rId86" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="O81" r:id="rId87" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="N82" r:id="rId88" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="O82" r:id="rId89" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="N83" r:id="rId90" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="O83" r:id="rId91" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="N84" r:id="rId92" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="O84" r:id="rId93" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="N85" r:id="rId94" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="O85" r:id="rId95" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="N86" r:id="rId96" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="O86" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="N87" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="O87" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="N88" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="O88" r:id="rId101" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="N89" r:id="rId102" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="O89" r:id="rId103" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="N90" r:id="rId104" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="O90" r:id="rId105" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="N91" r:id="rId106" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="O91" r:id="rId107" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="N92" r:id="rId108" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="O92" r:id="rId109" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="N93" r:id="rId110" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="O93" r:id="rId111" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="N94" r:id="rId112" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="O94" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="N95" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="O95" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="N96" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="O96" r:id="rId117" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="N97" r:id="rId118" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="O97" r:id="rId119" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="N98" r:id="rId120" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="O98" r:id="rId121" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="N112" r:id="rId122" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="N113" r:id="rId123" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="N114" r:id="rId124" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="N73" r:id="rId125" xr:uid="{9AF6E984-1653-430E-A3FB-A3D26D9878D9}"/>
+    <hyperlink ref="N99:N101" r:id="rId126" display="https://orcid.org/0000-0002-3380-3470" xr:uid="{C0237BC4-BA79-4297-A3EA-35626BCC8ACE}"/>
+    <hyperlink ref="N66:N69" r:id="rId127" display="https://orcid.org/0000-0002-3380-3470" xr:uid="{705A572F-F571-4480-A1DC-8DBA00CA101F}"/>
+    <hyperlink ref="N64" r:id="rId128" xr:uid="{1B7D45FB-4ED7-4ED1-BBC7-821751CC3EB3}"/>
+    <hyperlink ref="N65" r:id="rId129" xr:uid="{226E8F98-6EA9-42BC-9935-B19751C3752C}"/>
+    <hyperlink ref="N74" r:id="rId130" xr:uid="{265B2C5B-2BD4-4B09-BF2D-1D182ADD6769}"/>
+    <hyperlink ref="B1" r:id="rId131" display="https://vocabulary" xr:uid="{06485AB1-398E-4F4B-B0F0-CA6796438A4C}"/>
+    <hyperlink ref="C2" r:id="rId132" display="https://vocabulary" xr:uid="{B4136D2F-73FD-43A0-9364-C288E1E30184}"/>
+    <hyperlink ref="C3" r:id="rId133" xr:uid="{E2784929-558F-4C03-B04D-40A8B2AE08F8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId134"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="48a2b2ea-4ae5-49be-a8c4-5009d504025a">
@@ -3658,6 +4203,15 @@
     <TaxCatchAll xmlns="7fcf429e-959f-41cd-b9fc-3fe372134937" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3910,20 +4464,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BC35E7A-1AF8-4A96-AC97-C8D582699722}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC81F36B-8C49-4A34-8033-560B108372C9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="48a2b2ea-4ae5-49be-a8c4-5009d504025a"/>
     <ds:schemaRef ds:uri="7fcf429e-959f-41cd-b9fc-3fe372134937"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BC35E7A-1AF8-4A96-AC97-C8D582699722}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
collected updates since summer 2023
Updates include:
* concepts for describing facilities.
* variables for persistent organic pollutants, halogenated organics, precipitation chemistry, and others needed for EBAS data.
* introduction of deprecated concepts
</commit_message>
<xml_diff>
--- a/ACTRIS_controlled_lists.xlsx
+++ b/ACTRIS_controlled_lists.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nilu365.sharepoint.com/sites/Project-ACTRIS/Shared Documents/WP2 - In-Situ/vocabulary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{BF389FC4-FC65-4BA5-9E28-BDD5C3511B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{987A924B-8114-4DC5-9C66-4329D06AE180}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{93146FD7-108F-426C-9D14-35CBAFC91ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5993944-6BE0-4A3D-B685-2D1B2DA73C3A}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="2985" windowWidth="38700" windowHeight="15435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="43515" windowHeight="19830" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="controlled-terminology" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="197">
   <si>
     <t xml:space="preserve">ConceptScheme URI </t>
   </si>
@@ -543,6 +543,84 @@
   </si>
   <si>
     <t>Digital object identifier representing all versions of a record. Here, record means consistent set of data submissions from an identified instrument type and model at an identified location. Used to identify all previous, current, and future versions of the record.</t>
+  </si>
+  <si>
+    <t>simulation chamber controlled lists</t>
+  </si>
+  <si>
+    <t>aerosol in situ controlled lists</t>
+  </si>
+  <si>
+    <t>cloud in situ controlled lists</t>
+  </si>
+  <si>
+    <t>use metadata</t>
+  </si>
+  <si>
+    <t>ACTRIS_ctrl_lists:usemetadata</t>
+  </si>
+  <si>
+    <t>reactive trace gas in situ controlled lists</t>
+  </si>
+  <si>
+    <t>aerosol remote sensing controlled lists</t>
+  </si>
+  <si>
+    <t>cloud remote sensing controlled lists</t>
+  </si>
+  <si>
+    <t>reactive trace gas remote sensing controlled lists</t>
+  </si>
+  <si>
+    <t>Controlled vocabulary for detailed descriptions of operating procedures.</t>
+  </si>
+  <si>
+    <t>simulation chamber light sources</t>
+  </si>
+  <si>
+    <t>dark chamber</t>
+  </si>
+  <si>
+    <t>fluorescent lamps</t>
+  </si>
+  <si>
+    <t>natural sunlight</t>
+  </si>
+  <si>
+    <t>other artificial light source</t>
+  </si>
+  <si>
+    <t>xenon arc lamps</t>
+  </si>
+  <si>
+    <t>ACTRIS_ctrl_lists:simulationchambercontrolledlists</t>
+  </si>
+  <si>
+    <t>ACTRIS_ctrl_lists:simulationchamberlightsources</t>
+  </si>
+  <si>
+    <t>simulation chamber wall types</t>
+  </si>
+  <si>
+    <t>FEP film</t>
+  </si>
+  <si>
+    <t>Pyrex</t>
+  </si>
+  <si>
+    <t>quartz</t>
+  </si>
+  <si>
+    <t>stainless steel</t>
+  </si>
+  <si>
+    <t>aluminium</t>
+  </si>
+  <si>
+    <t>fluorinated ethylene propylene film</t>
+  </si>
+  <si>
+    <t>ACTRIS_ctrl_lists:simulationchamberwalltypes</t>
   </si>
   <si>
     <t>https://vocabulary.actris.nilu.no/actris_controlled_lists/</t>
@@ -1179,12 +1257,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P115"/>
+  <dimension ref="A1:P154"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A1771" sqref="A1771"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3:C3"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1208,7 +1286,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>169</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -1219,7 +1297,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>169</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -1230,7 +1308,7 @@
         <v>151</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -3635,7 +3713,7 @@
     </row>
     <row r="98" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="15" t="str">
-        <f t="shared" ref="A98:A115" si="4">IF(ISBLANK($B98),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B98," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <f t="shared" ref="A98:A129" si="4">IF(ISBLANK($B98),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B98," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
         <v>ACTRIS_ctrl_lists:NOAA-ESRL</v>
       </c>
       <c r="B98" s="17" t="s">
@@ -3943,11 +4021,15 @@
     <row r="111" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="12" t="str">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="B111" s="13"/>
+        <v>ACTRIS_ctrl_lists:usemetadata</v>
+      </c>
+      <c r="B111" s="13" t="s">
+        <v>172</v>
+      </c>
       <c r="C111" s="13"/>
-      <c r="D111" s="13"/>
+      <c r="D111" s="13" t="s">
+        <v>178</v>
+      </c>
       <c r="E111" s="13"/>
       <c r="F111" s="13"/>
       <c r="G111" s="13"/>
@@ -3966,12 +4048,16 @@
     <row r="112" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="24" t="str">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="B112" s="25"/>
+        <v>ACTRIS_ctrl_lists:simulationchambercontrolledlists</v>
+      </c>
+      <c r="B112" s="25" t="s">
+        <v>169</v>
+      </c>
       <c r="C112" s="25"/>
       <c r="D112" s="25"/>
-      <c r="E112" s="25"/>
+      <c r="E112" s="25" t="s">
+        <v>173</v>
+      </c>
       <c r="F112" s="25"/>
       <c r="G112" s="25"/>
       <c r="H112" s="25"/>
@@ -3989,12 +4075,16 @@
     <row r="113" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="27" t="str">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="B113" s="28"/>
+        <v>ACTRIS_ctrl_lists:simulationchamberlightsources</v>
+      </c>
+      <c r="B113" s="28" t="s">
+        <v>179</v>
+      </c>
       <c r="C113" s="28"/>
       <c r="D113" s="28"/>
-      <c r="E113" s="28"/>
+      <c r="E113" s="28" t="s">
+        <v>185</v>
+      </c>
       <c r="F113" s="28"/>
       <c r="G113" s="28"/>
       <c r="H113" s="28"/>
@@ -4012,12 +4102,16 @@
     <row r="114" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="15" t="str">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="B114" s="17"/>
+        <v>ACTRIS_ctrl_lists:darkchamber</v>
+      </c>
+      <c r="B114" s="17" t="s">
+        <v>180</v>
+      </c>
       <c r="C114" s="18"/>
       <c r="D114" s="17"/>
-      <c r="E114" s="17"/>
+      <c r="E114" s="18" t="s">
+        <v>186</v>
+      </c>
       <c r="F114" s="18"/>
       <c r="G114" s="18"/>
       <c r="H114" s="18"/>
@@ -4035,12 +4129,16 @@
     <row r="115" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="15" t="str">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="B115" s="18"/>
+        <v>ACTRIS_ctrl_lists:fluorescentlamps</v>
+      </c>
+      <c r="B115" s="17" t="s">
+        <v>181</v>
+      </c>
       <c r="C115" s="18"/>
       <c r="D115" s="17"/>
-      <c r="E115" s="17"/>
+      <c r="E115" s="18" t="s">
+        <v>186</v>
+      </c>
       <c r="F115" s="18"/>
       <c r="G115" s="18"/>
       <c r="H115" s="18"/>
@@ -4049,9 +4147,920 @@
       <c r="K115" s="18"/>
       <c r="L115" s="18"/>
       <c r="M115" s="18"/>
-      <c r="N115" s="23"/>
+      <c r="N115" s="23" t="s">
+        <v>44</v>
+      </c>
       <c r="O115" s="23"/>
       <c r="P115" s="18"/>
+    </row>
+    <row r="116" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v>ACTRIS_ctrl_lists:naturalsunlight</v>
+      </c>
+      <c r="B116" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="C116" s="18"/>
+      <c r="D116" s="17"/>
+      <c r="E116" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="F116" s="18"/>
+      <c r="G116" s="18"/>
+      <c r="H116" s="18"/>
+      <c r="I116" s="18"/>
+      <c r="J116" s="18"/>
+      <c r="K116" s="18"/>
+      <c r="L116" s="18"/>
+      <c r="M116" s="18"/>
+      <c r="N116" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="O116" s="23"/>
+      <c r="P116" s="18"/>
+    </row>
+    <row r="117" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v>ACTRIS_ctrl_lists:otherartificiallightsource</v>
+      </c>
+      <c r="B117" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="C117" s="18"/>
+      <c r="D117" s="17"/>
+      <c r="E117" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="F117" s="18"/>
+      <c r="G117" s="18"/>
+      <c r="H117" s="18"/>
+      <c r="I117" s="18"/>
+      <c r="J117" s="18"/>
+      <c r="K117" s="18"/>
+      <c r="L117" s="18"/>
+      <c r="M117" s="18"/>
+      <c r="N117" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="O117" s="23"/>
+      <c r="P117" s="18"/>
+    </row>
+    <row r="118" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v>ACTRIS_ctrl_lists:xenonarclamps</v>
+      </c>
+      <c r="B118" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="C118" s="18"/>
+      <c r="D118" s="17"/>
+      <c r="E118" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="F118" s="18"/>
+      <c r="G118" s="18"/>
+      <c r="H118" s="18"/>
+      <c r="I118" s="18"/>
+      <c r="J118" s="18"/>
+      <c r="K118" s="18"/>
+      <c r="L118" s="18"/>
+      <c r="M118" s="18"/>
+      <c r="N118" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="O118" s="23"/>
+      <c r="P118" s="18"/>
+    </row>
+    <row r="119" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B119" s="17"/>
+      <c r="C119" s="18"/>
+      <c r="D119" s="17"/>
+      <c r="E119" s="18"/>
+      <c r="F119" s="18"/>
+      <c r="G119" s="18"/>
+      <c r="H119" s="18"/>
+      <c r="I119" s="18"/>
+      <c r="J119" s="18"/>
+      <c r="K119" s="18"/>
+      <c r="L119" s="18"/>
+      <c r="M119" s="18"/>
+      <c r="N119" s="23"/>
+      <c r="O119" s="23"/>
+      <c r="P119" s="18"/>
+    </row>
+    <row r="120" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="27" t="str">
+        <f t="shared" ref="A120" si="6">IF(ISBLANK($B120),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B120," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <v>ACTRIS_ctrl_lists:simulationchamberwalltypes</v>
+      </c>
+      <c r="B120" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="C120" s="28"/>
+      <c r="D120" s="28"/>
+      <c r="E120" s="28" t="s">
+        <v>185</v>
+      </c>
+      <c r="F120" s="28"/>
+      <c r="G120" s="28"/>
+      <c r="H120" s="28"/>
+      <c r="I120" s="28"/>
+      <c r="J120" s="28"/>
+      <c r="K120" s="28"/>
+      <c r="L120" s="28"/>
+      <c r="M120" s="28"/>
+      <c r="N120" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="O120" s="28"/>
+      <c r="P120" s="28"/>
+    </row>
+    <row r="121" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v>ACTRIS_ctrl_lists:aluminium</v>
+      </c>
+      <c r="B121" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="C121" s="18"/>
+      <c r="D121" s="17"/>
+      <c r="E121" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="F121" s="18"/>
+      <c r="G121" s="18"/>
+      <c r="H121" s="18"/>
+      <c r="I121" s="18"/>
+      <c r="J121" s="18"/>
+      <c r="K121" s="18"/>
+      <c r="L121" s="18"/>
+      <c r="M121" s="18"/>
+      <c r="N121" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="O121" s="23"/>
+      <c r="P121" s="18"/>
+    </row>
+    <row r="122" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v>ACTRIS_ctrl_lists:fluorinatedethylenepropylenefilm</v>
+      </c>
+      <c r="B122" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="C122" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="D122" s="17"/>
+      <c r="E122" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="F122" s="18"/>
+      <c r="G122" s="18"/>
+      <c r="H122" s="18"/>
+      <c r="I122" s="18"/>
+      <c r="J122" s="18"/>
+      <c r="K122" s="18"/>
+      <c r="L122" s="18"/>
+      <c r="M122" s="18"/>
+      <c r="N122" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="O122" s="23"/>
+      <c r="P122" s="18"/>
+    </row>
+    <row r="123" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v>ACTRIS_ctrl_lists:Pyrex</v>
+      </c>
+      <c r="B123" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="C123" s="18"/>
+      <c r="D123" s="17"/>
+      <c r="E123" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="F123" s="18"/>
+      <c r="G123" s="18"/>
+      <c r="H123" s="18"/>
+      <c r="I123" s="18"/>
+      <c r="J123" s="18"/>
+      <c r="K123" s="18"/>
+      <c r="L123" s="18"/>
+      <c r="M123" s="18"/>
+      <c r="N123" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="O123" s="23"/>
+      <c r="P123" s="18"/>
+    </row>
+    <row r="124" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v>ACTRIS_ctrl_lists:quartz</v>
+      </c>
+      <c r="B124" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="C124" s="18"/>
+      <c r="D124" s="17"/>
+      <c r="E124" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="F124" s="18"/>
+      <c r="G124" s="18"/>
+      <c r="H124" s="18"/>
+      <c r="I124" s="18"/>
+      <c r="J124" s="18"/>
+      <c r="K124" s="18"/>
+      <c r="L124" s="18"/>
+      <c r="M124" s="18"/>
+      <c r="N124" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="O124" s="23"/>
+      <c r="P124" s="18"/>
+    </row>
+    <row r="125" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v>ACTRIS_ctrl_lists:stainlesssteel</v>
+      </c>
+      <c r="B125" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="C125" s="18"/>
+      <c r="D125" s="17"/>
+      <c r="E125" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="F125" s="18"/>
+      <c r="G125" s="18"/>
+      <c r="H125" s="18"/>
+      <c r="I125" s="18"/>
+      <c r="J125" s="18"/>
+      <c r="K125" s="18"/>
+      <c r="L125" s="18"/>
+      <c r="M125" s="18"/>
+      <c r="N125" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="O125" s="23"/>
+      <c r="P125" s="18"/>
+    </row>
+    <row r="126" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B126" s="17"/>
+      <c r="C126" s="18"/>
+      <c r="D126" s="17"/>
+      <c r="E126" s="18"/>
+      <c r="F126" s="18"/>
+      <c r="G126" s="18"/>
+      <c r="H126" s="18"/>
+      <c r="I126" s="18"/>
+      <c r="J126" s="18"/>
+      <c r="K126" s="18"/>
+      <c r="L126" s="18"/>
+      <c r="M126" s="18"/>
+      <c r="N126" s="23"/>
+      <c r="O126" s="23"/>
+      <c r="P126" s="18"/>
+    </row>
+    <row r="127" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="15" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B127" s="17"/>
+      <c r="C127" s="18"/>
+      <c r="D127" s="17"/>
+      <c r="E127" s="18"/>
+      <c r="F127" s="18"/>
+      <c r="G127" s="18"/>
+      <c r="H127" s="18"/>
+      <c r="I127" s="18"/>
+      <c r="J127" s="18"/>
+      <c r="K127" s="18"/>
+      <c r="L127" s="18"/>
+      <c r="M127" s="18"/>
+      <c r="N127" s="23"/>
+      <c r="O127" s="23"/>
+      <c r="P127" s="18"/>
+    </row>
+    <row r="128" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A128" s="24" t="str">
+        <f t="shared" si="4"/>
+        <v>ACTRIS_ctrl_lists:aerosolinsitucontrolledlists</v>
+      </c>
+      <c r="B128" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="C128" s="25"/>
+      <c r="D128" s="25"/>
+      <c r="E128" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="F128" s="25"/>
+      <c r="G128" s="25"/>
+      <c r="H128" s="25"/>
+      <c r="I128" s="25"/>
+      <c r="J128" s="25"/>
+      <c r="K128" s="25"/>
+      <c r="L128" s="25"/>
+      <c r="M128" s="25"/>
+      <c r="N128" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="O128" s="25"/>
+      <c r="P128" s="25"/>
+    </row>
+    <row r="129" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="27" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B129" s="28"/>
+      <c r="C129" s="28"/>
+      <c r="D129" s="28"/>
+      <c r="E129" s="28"/>
+      <c r="F129" s="28"/>
+      <c r="G129" s="28"/>
+      <c r="H129" s="28"/>
+      <c r="I129" s="28"/>
+      <c r="J129" s="28"/>
+      <c r="K129" s="28"/>
+      <c r="L129" s="28"/>
+      <c r="M129" s="28"/>
+      <c r="N129" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="O129" s="28"/>
+      <c r="P129" s="28"/>
+    </row>
+    <row r="130" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="15"/>
+      <c r="B130" s="17"/>
+      <c r="C130" s="18"/>
+      <c r="D130" s="17"/>
+      <c r="E130" s="18"/>
+      <c r="F130" s="18"/>
+      <c r="G130" s="18"/>
+      <c r="H130" s="18"/>
+      <c r="I130" s="18"/>
+      <c r="J130" s="18"/>
+      <c r="K130" s="18"/>
+      <c r="L130" s="18"/>
+      <c r="M130" s="18"/>
+      <c r="N130" s="23"/>
+      <c r="O130" s="23"/>
+      <c r="P130" s="18"/>
+    </row>
+    <row r="131" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="24" t="str">
+        <f t="shared" ref="A131:A132" si="7">IF(ISBLANK($B131),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B131," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <v>ACTRIS_ctrl_lists:cloudinsitucontrolledlists</v>
+      </c>
+      <c r="B131" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="C131" s="25"/>
+      <c r="D131" s="25"/>
+      <c r="E131" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="F131" s="25"/>
+      <c r="G131" s="25"/>
+      <c r="H131" s="25"/>
+      <c r="I131" s="25"/>
+      <c r="J131" s="25"/>
+      <c r="K131" s="25"/>
+      <c r="L131" s="25"/>
+      <c r="M131" s="25"/>
+      <c r="N131" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="O131" s="25"/>
+      <c r="P131" s="25"/>
+    </row>
+    <row r="132" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="27" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="B132" s="28"/>
+      <c r="C132" s="28"/>
+      <c r="D132" s="28"/>
+      <c r="E132" s="28"/>
+      <c r="F132" s="28"/>
+      <c r="G132" s="28"/>
+      <c r="H132" s="28"/>
+      <c r="I132" s="28"/>
+      <c r="J132" s="28"/>
+      <c r="K132" s="28"/>
+      <c r="L132" s="28"/>
+      <c r="M132" s="28"/>
+      <c r="N132" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="O132" s="28"/>
+      <c r="P132" s="28"/>
+    </row>
+    <row r="133" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A133" s="15"/>
+      <c r="B133" s="17"/>
+      <c r="C133" s="18"/>
+      <c r="D133" s="17"/>
+      <c r="E133" s="18"/>
+      <c r="F133" s="18"/>
+      <c r="G133" s="18"/>
+      <c r="H133" s="18"/>
+      <c r="I133" s="18"/>
+      <c r="J133" s="18"/>
+      <c r="K133" s="18"/>
+      <c r="L133" s="18"/>
+      <c r="M133" s="18"/>
+      <c r="N133" s="23"/>
+      <c r="O133" s="23"/>
+      <c r="P133" s="18"/>
+    </row>
+    <row r="134" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="15"/>
+      <c r="B134" s="17"/>
+      <c r="C134" s="18"/>
+      <c r="D134" s="17"/>
+      <c r="E134" s="18"/>
+      <c r="F134" s="18"/>
+      <c r="G134" s="18"/>
+      <c r="H134" s="18"/>
+      <c r="I134" s="18"/>
+      <c r="J134" s="18"/>
+      <c r="K134" s="18"/>
+      <c r="L134" s="18"/>
+      <c r="M134" s="18"/>
+      <c r="N134" s="23"/>
+      <c r="O134" s="23"/>
+      <c r="P134" s="18"/>
+    </row>
+    <row r="135" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="24" t="str">
+        <f t="shared" ref="A135:A136" si="8">IF(ISBLANK($B135),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B135," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <v>ACTRIS_ctrl_lists:reactivetracegasinsitucontrolledlists</v>
+      </c>
+      <c r="B135" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="C135" s="25"/>
+      <c r="D135" s="25"/>
+      <c r="E135" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="F135" s="25"/>
+      <c r="G135" s="25"/>
+      <c r="H135" s="25"/>
+      <c r="I135" s="25"/>
+      <c r="J135" s="25"/>
+      <c r="K135" s="25"/>
+      <c r="L135" s="25"/>
+      <c r="M135" s="25"/>
+      <c r="N135" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="O135" s="25"/>
+      <c r="P135" s="25"/>
+    </row>
+    <row r="136" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A136" s="27" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="B136" s="28"/>
+      <c r="C136" s="28"/>
+      <c r="D136" s="28"/>
+      <c r="E136" s="28"/>
+      <c r="F136" s="28"/>
+      <c r="G136" s="28"/>
+      <c r="H136" s="28"/>
+      <c r="I136" s="28"/>
+      <c r="J136" s="28"/>
+      <c r="K136" s="28"/>
+      <c r="L136" s="28"/>
+      <c r="M136" s="28"/>
+      <c r="N136" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="O136" s="28"/>
+      <c r="P136" s="28"/>
+    </row>
+    <row r="137" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A137" s="15"/>
+      <c r="B137" s="17"/>
+      <c r="C137" s="18"/>
+      <c r="D137" s="17"/>
+      <c r="E137" s="18"/>
+      <c r="F137" s="18"/>
+      <c r="G137" s="18"/>
+      <c r="H137" s="18"/>
+      <c r="I137" s="18"/>
+      <c r="J137" s="18"/>
+      <c r="K137" s="18"/>
+      <c r="L137" s="18"/>
+      <c r="M137" s="18"/>
+      <c r="N137" s="23"/>
+      <c r="O137" s="23"/>
+      <c r="P137" s="18"/>
+    </row>
+    <row r="138" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A138" s="15"/>
+      <c r="B138" s="17"/>
+      <c r="C138" s="18"/>
+      <c r="D138" s="17"/>
+      <c r="E138" s="18"/>
+      <c r="F138" s="18"/>
+      <c r="G138" s="18"/>
+      <c r="H138" s="18"/>
+      <c r="I138" s="18"/>
+      <c r="J138" s="18"/>
+      <c r="K138" s="18"/>
+      <c r="L138" s="18"/>
+      <c r="M138" s="18"/>
+      <c r="N138" s="23"/>
+      <c r="O138" s="23"/>
+      <c r="P138" s="18"/>
+    </row>
+    <row r="139" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A139" s="24" t="str">
+        <f t="shared" ref="A139:A140" si="9">IF(ISBLANK($B139),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B139," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <v>ACTRIS_ctrl_lists:aerosolremotesensingcontrolledlists</v>
+      </c>
+      <c r="B139" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="C139" s="25"/>
+      <c r="D139" s="25"/>
+      <c r="E139" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="F139" s="25"/>
+      <c r="G139" s="25"/>
+      <c r="H139" s="25"/>
+      <c r="I139" s="25"/>
+      <c r="J139" s="25"/>
+      <c r="K139" s="25"/>
+      <c r="L139" s="25"/>
+      <c r="M139" s="25"/>
+      <c r="N139" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="O139" s="25"/>
+      <c r="P139" s="25"/>
+    </row>
+    <row r="140" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A140" s="27" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="B140" s="28"/>
+      <c r="C140" s="28"/>
+      <c r="D140" s="28"/>
+      <c r="E140" s="28"/>
+      <c r="F140" s="28"/>
+      <c r="G140" s="28"/>
+      <c r="H140" s="28"/>
+      <c r="I140" s="28"/>
+      <c r="J140" s="28"/>
+      <c r="K140" s="28"/>
+      <c r="L140" s="28"/>
+      <c r="M140" s="28"/>
+      <c r="N140" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="O140" s="28"/>
+      <c r="P140" s="28"/>
+    </row>
+    <row r="141" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A141" s="15"/>
+      <c r="B141" s="17"/>
+      <c r="C141" s="18"/>
+      <c r="D141" s="17"/>
+      <c r="E141" s="18"/>
+      <c r="F141" s="18"/>
+      <c r="G141" s="18"/>
+      <c r="H141" s="18"/>
+      <c r="I141" s="18"/>
+      <c r="J141" s="18"/>
+      <c r="K141" s="18"/>
+      <c r="L141" s="18"/>
+      <c r="M141" s="18"/>
+      <c r="N141" s="23"/>
+      <c r="O141" s="23"/>
+      <c r="P141" s="18"/>
+    </row>
+    <row r="142" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A142" s="15"/>
+      <c r="B142" s="17"/>
+      <c r="C142" s="18"/>
+      <c r="D142" s="17"/>
+      <c r="E142" s="18"/>
+      <c r="F142" s="18"/>
+      <c r="G142" s="18"/>
+      <c r="H142" s="18"/>
+      <c r="I142" s="18"/>
+      <c r="J142" s="18"/>
+      <c r="K142" s="18"/>
+      <c r="L142" s="18"/>
+      <c r="M142" s="18"/>
+      <c r="N142" s="23"/>
+      <c r="O142" s="23"/>
+      <c r="P142" s="18"/>
+    </row>
+    <row r="143" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A143" s="24" t="str">
+        <f t="shared" ref="A143:A144" si="10">IF(ISBLANK($B143),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B143," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <v>ACTRIS_ctrl_lists:cloudremotesensingcontrolledlists</v>
+      </c>
+      <c r="B143" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="C143" s="25"/>
+      <c r="D143" s="25"/>
+      <c r="E143" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="F143" s="25"/>
+      <c r="G143" s="25"/>
+      <c r="H143" s="25"/>
+      <c r="I143" s="25"/>
+      <c r="J143" s="25"/>
+      <c r="K143" s="25"/>
+      <c r="L143" s="25"/>
+      <c r="M143" s="25"/>
+      <c r="N143" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="O143" s="25"/>
+      <c r="P143" s="25"/>
+    </row>
+    <row r="144" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A144" s="27" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="B144" s="28"/>
+      <c r="C144" s="28"/>
+      <c r="D144" s="28"/>
+      <c r="E144" s="28"/>
+      <c r="F144" s="28"/>
+      <c r="G144" s="28"/>
+      <c r="H144" s="28"/>
+      <c r="I144" s="28"/>
+      <c r="J144" s="28"/>
+      <c r="K144" s="28"/>
+      <c r="L144" s="28"/>
+      <c r="M144" s="28"/>
+      <c r="N144" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="O144" s="28"/>
+      <c r="P144" s="28"/>
+    </row>
+    <row r="145" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A145" s="15"/>
+      <c r="B145" s="17"/>
+      <c r="C145" s="18"/>
+      <c r="D145" s="17"/>
+      <c r="E145" s="18"/>
+      <c r="F145" s="18"/>
+      <c r="G145" s="18"/>
+      <c r="H145" s="18"/>
+      <c r="I145" s="18"/>
+      <c r="J145" s="18"/>
+      <c r="K145" s="18"/>
+      <c r="L145" s="18"/>
+      <c r="M145" s="18"/>
+      <c r="N145" s="23"/>
+      <c r="O145" s="23"/>
+      <c r="P145" s="18"/>
+    </row>
+    <row r="146" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A146" s="24" t="str">
+        <f t="shared" ref="A146:A147" si="11">IF(ISBLANK($B146),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B146," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <v>ACTRIS_ctrl_lists:reactivetracegasremotesensingcontrolledlists</v>
+      </c>
+      <c r="B146" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="C146" s="25"/>
+      <c r="D146" s="25"/>
+      <c r="E146" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="F146" s="25"/>
+      <c r="G146" s="25"/>
+      <c r="H146" s="25"/>
+      <c r="I146" s="25"/>
+      <c r="J146" s="25"/>
+      <c r="K146" s="25"/>
+      <c r="L146" s="25"/>
+      <c r="M146" s="25"/>
+      <c r="N146" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="O146" s="25"/>
+      <c r="P146" s="25"/>
+    </row>
+    <row r="147" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A147" s="27" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="B147" s="28"/>
+      <c r="C147" s="28"/>
+      <c r="D147" s="28"/>
+      <c r="E147" s="28"/>
+      <c r="F147" s="28"/>
+      <c r="G147" s="28"/>
+      <c r="H147" s="28"/>
+      <c r="I147" s="28"/>
+      <c r="J147" s="28"/>
+      <c r="K147" s="28"/>
+      <c r="L147" s="28"/>
+      <c r="M147" s="28"/>
+      <c r="N147" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="O147" s="28"/>
+      <c r="P147" s="28"/>
+    </row>
+    <row r="148" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A148" s="15" t="str">
+        <f t="shared" ref="A148:A154" si="12">IF(ISBLANK($B148),"",$B$2 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B148," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <v/>
+      </c>
+      <c r="B148" s="17"/>
+      <c r="C148" s="18"/>
+      <c r="D148" s="17"/>
+      <c r="E148" s="17"/>
+      <c r="F148" s="18"/>
+      <c r="G148" s="18"/>
+      <c r="H148" s="18"/>
+      <c r="I148" s="18"/>
+      <c r="J148" s="18"/>
+      <c r="K148" s="18"/>
+      <c r="L148" s="18"/>
+      <c r="M148" s="18"/>
+      <c r="N148" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="O148" s="23"/>
+      <c r="P148" s="18"/>
+    </row>
+    <row r="149" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A149" s="15" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="B149" s="18"/>
+      <c r="C149" s="18"/>
+      <c r="D149" s="17"/>
+      <c r="E149" s="17"/>
+      <c r="F149" s="18"/>
+      <c r="G149" s="18"/>
+      <c r="H149" s="18"/>
+      <c r="I149" s="18"/>
+      <c r="J149" s="18"/>
+      <c r="K149" s="18"/>
+      <c r="L149" s="18"/>
+      <c r="M149" s="18"/>
+      <c r="N149" s="23"/>
+      <c r="O149" s="23"/>
+      <c r="P149" s="18"/>
+    </row>
+    <row r="150" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A150" s="12" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="B150" s="13"/>
+      <c r="C150" s="13"/>
+      <c r="D150" s="13"/>
+      <c r="E150" s="13"/>
+      <c r="F150" s="13"/>
+      <c r="G150" s="13"/>
+      <c r="H150" s="13"/>
+      <c r="I150" s="13"/>
+      <c r="J150" s="13"/>
+      <c r="K150" s="13"/>
+      <c r="L150" s="13"/>
+      <c r="M150" s="13"/>
+      <c r="N150" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="O150" s="13"/>
+      <c r="P150" s="13"/>
+    </row>
+    <row r="151" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A151" s="24" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="B151" s="25"/>
+      <c r="C151" s="25"/>
+      <c r="D151" s="25"/>
+      <c r="E151" s="25"/>
+      <c r="F151" s="25"/>
+      <c r="G151" s="25"/>
+      <c r="H151" s="25"/>
+      <c r="I151" s="25"/>
+      <c r="J151" s="25"/>
+      <c r="K151" s="25"/>
+      <c r="L151" s="25"/>
+      <c r="M151" s="25"/>
+      <c r="N151" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="O151" s="25"/>
+      <c r="P151" s="25"/>
+    </row>
+    <row r="152" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A152" s="27" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="B152" s="28"/>
+      <c r="C152" s="28"/>
+      <c r="D152" s="28"/>
+      <c r="E152" s="28"/>
+      <c r="F152" s="28"/>
+      <c r="G152" s="28"/>
+      <c r="H152" s="28"/>
+      <c r="I152" s="28"/>
+      <c r="J152" s="28"/>
+      <c r="K152" s="28"/>
+      <c r="L152" s="28"/>
+      <c r="M152" s="28"/>
+      <c r="N152" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="O152" s="28"/>
+      <c r="P152" s="28"/>
+    </row>
+    <row r="153" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A153" s="15" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="B153" s="17"/>
+      <c r="C153" s="18"/>
+      <c r="D153" s="17"/>
+      <c r="E153" s="17"/>
+      <c r="F153" s="18"/>
+      <c r="G153" s="18"/>
+      <c r="H153" s="18"/>
+      <c r="I153" s="18"/>
+      <c r="J153" s="18"/>
+      <c r="K153" s="18"/>
+      <c r="L153" s="18"/>
+      <c r="M153" s="18"/>
+      <c r="N153" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="O153" s="23"/>
+      <c r="P153" s="18"/>
+    </row>
+    <row r="154" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A154" s="15" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="B154" s="18"/>
+      <c r="C154" s="18"/>
+      <c r="D154" s="17"/>
+      <c r="E154" s="17"/>
+      <c r="F154" s="18"/>
+      <c r="G154" s="18"/>
+      <c r="H154" s="18"/>
+      <c r="I154" s="18"/>
+      <c r="J154" s="18"/>
+      <c r="K154" s="18"/>
+      <c r="L154" s="18"/>
+      <c r="M154" s="18"/>
+      <c r="N154" s="23"/>
+      <c r="O154" s="23"/>
+      <c r="P154" s="18"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4185,36 +5194,35 @@
     <hyperlink ref="N64" r:id="rId128" xr:uid="{1B7D45FB-4ED7-4ED1-BBC7-821751CC3EB3}"/>
     <hyperlink ref="N65" r:id="rId129" xr:uid="{226E8F98-6EA9-42BC-9935-B19751C3752C}"/>
     <hyperlink ref="N74" r:id="rId130" xr:uid="{265B2C5B-2BD4-4B09-BF2D-1D182ADD6769}"/>
-    <hyperlink ref="B1" r:id="rId131" display="https://vocabulary" xr:uid="{06485AB1-398E-4F4B-B0F0-CA6796438A4C}"/>
-    <hyperlink ref="C2" r:id="rId132" display="https://vocabulary" xr:uid="{B4136D2F-73FD-43A0-9364-C288E1E30184}"/>
-    <hyperlink ref="C3" r:id="rId133" xr:uid="{E2784929-558F-4C03-B04D-40A8B2AE08F8}"/>
+    <hyperlink ref="N148" r:id="rId131" xr:uid="{BFA3A315-68ED-41AC-A422-E5B270BCAA65}"/>
+    <hyperlink ref="N151" r:id="rId132" xr:uid="{EF50E818-5C00-457D-A67A-B09335A7D545}"/>
+    <hyperlink ref="N152" r:id="rId133" xr:uid="{7271C232-2EEF-47E3-BD2F-E8FCA1B9195C}"/>
+    <hyperlink ref="N153" r:id="rId134" xr:uid="{9B567F81-6F3A-4D2A-B380-E99564D4295D}"/>
+    <hyperlink ref="N128" r:id="rId135" xr:uid="{BEAB9E3F-2C94-4909-9BE6-8DF462A2C30F}"/>
+    <hyperlink ref="N129" r:id="rId136" xr:uid="{111B9A1B-3F82-4F34-9566-46C7A83C04DB}"/>
+    <hyperlink ref="N131" r:id="rId137" xr:uid="{612D57F9-55A6-4BFA-B2C5-222EFEB10181}"/>
+    <hyperlink ref="N132" r:id="rId138" xr:uid="{2354DB23-F51A-45D0-8DC0-494B9A9E76F1}"/>
+    <hyperlink ref="N135" r:id="rId139" xr:uid="{864B7DC4-2B18-48D9-A771-D5C980DC5D0F}"/>
+    <hyperlink ref="N136" r:id="rId140" xr:uid="{76D79C66-0314-4400-BA60-9A4924CE1344}"/>
+    <hyperlink ref="N139" r:id="rId141" xr:uid="{CBDAF360-DD30-4FFE-9873-8D715A36F95E}"/>
+    <hyperlink ref="N140" r:id="rId142" xr:uid="{78708F00-E983-42F1-AD4A-F42143EE0641}"/>
+    <hyperlink ref="N143" r:id="rId143" xr:uid="{0C8BD3CC-3F65-4CDB-9F7F-68AE696A848E}"/>
+    <hyperlink ref="N144" r:id="rId144" xr:uid="{718F6210-5612-476D-BD89-516382F3AC7B}"/>
+    <hyperlink ref="N146" r:id="rId145" xr:uid="{D72136AE-8722-4F19-B815-D2BC69B3790F}"/>
+    <hyperlink ref="N147" r:id="rId146" xr:uid="{63035A47-7690-4D5B-83D1-48366F2115A7}"/>
+    <hyperlink ref="N120" r:id="rId147" xr:uid="{DB3FA559-07DB-4E3F-8F33-03E67AA6594B}"/>
+    <hyperlink ref="N115:N118" r:id="rId148" display="https://orcid.org/0000-0002-3380-3470" xr:uid="{3B067DB1-3926-4DF6-B802-C6C41B490EE4}"/>
+    <hyperlink ref="N121:N125" r:id="rId149" display="https://orcid.org/0000-0002-3380-3470" xr:uid="{72F1B155-0CBB-46FF-8205-A0C52E9A070F}"/>
+    <hyperlink ref="B1" r:id="rId150" display="https://vocabulary" xr:uid="{FC63CCF7-4106-4079-8897-D7CC351A83D3}"/>
+    <hyperlink ref="C2" r:id="rId151" display="https://vocabulary" xr:uid="{7615EF84-DACB-45A1-A935-6A8D56510439}"/>
+    <hyperlink ref="C3" r:id="rId152" xr:uid="{27AAFF6E-A340-46E6-802E-D730F8B28349}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId134"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId153"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="48a2b2ea-4ae5-49be-a8c4-5009d504025a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7fcf429e-959f-41cd-b9fc-3fe372134937" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006481788B230DB442BDFB5C65881F7436" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d0b37471ba0f4334be182783e7df3327">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="48a2b2ea-4ae5-49be-a8c4-5009d504025a" xmlns:ns3="7fcf429e-959f-41cd-b9fc-3fe372134937" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7fdc9a5503b4fe454d295efe7f1cb2ee" ns2:_="" ns3:_="">
     <xsd:import namespace="48a2b2ea-4ae5-49be-a8c4-5009d504025a"/>
@@ -4463,26 +5471,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC81F36B-8C49-4A34-8033-560B108372C9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="48a2b2ea-4ae5-49be-a8c4-5009d504025a"/>
-    <ds:schemaRef ds:uri="7fcf429e-959f-41cd-b9fc-3fe372134937"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="48a2b2ea-4ae5-49be-a8c4-5009d504025a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7fcf429e-959f-41cd-b9fc-3fe372134937" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BC35E7A-1AF8-4A96-AC97-C8D582699722}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D333BA1-2FD2-47F6-8B16-E090A3639941}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4499,4 +5508,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC81F36B-8C49-4A34-8033-560B108372C9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="48a2b2ea-4ae5-49be-a8c4-5009d504025a"/>
+    <ds:schemaRef ds:uri="7fcf429e-959f-41cd-b9fc-3fe372134937"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BC35E7A-1AF8-4A96-AC97-C8D582699722}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>